<commit_message>
MAJ LIEN COUDES CARREES ET PLANS INCONNUS TRANSFO CC ET RC
</commit_message>
<xml_diff>
--- a/Remote/Commun/dist_liens.xlsx
+++ b/Remote/Commun/dist_liens.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Mickaël\Documents\GitHub\ductaironline\ductaironline\Remote\Commun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01EBA892-DB2F-4D0F-BB8C-2C96B198F097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D53AF91-7CC1-4E3C-B08C-8D4112A2BBBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{10E80606-BDFD-48EA-859F-8B282D217FD1}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="dist_liens" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">dist_liens!$C$1:$V$169</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">dist_liens!$C$1:$V$173</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3375" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3445" uniqueCount="259">
   <si>
     <t>id</t>
   </si>
@@ -449,12 +449,6 @@
     <t>A2</t>
   </si>
   <si>
-    <t>B2</t>
-  </si>
-  <si>
-    <t>F2</t>
-  </si>
-  <si>
     <t>00/00/0001</t>
   </si>
   <si>
@@ -804,6 +798,24 @@
   </si>
   <si>
     <t>2p</t>
+  </si>
+  <si>
+    <t>EEG</t>
+  </si>
+  <si>
+    <t>REG</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Drawings/C/C90/EQUERRE/C90carre.jpg</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Drawings/C/C90/RAYON/C90carre.jpg</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Drawings/C/C45/EQUERRE/C45carre.jpg</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Drawings/C/C45/RAYON/C45carre.jpg</t>
   </si>
 </sst>
 </file>
@@ -1212,11 +1224,11 @@
   <sheetPr codeName="Feuil36">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CD169"/>
+  <dimension ref="A1:CD173"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="K88" sqref="K88:R121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2051,7 +2063,7 @@
         <v>28</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F4" t="s">
         <v>46</v>
@@ -2547,7 +2559,7 @@
         <v>28</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F6" t="s">
         <v>48</v>
@@ -3542,7 +3554,7 @@
         <v>29</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G10">
         <v>120</v>
@@ -4035,7 +4047,7 @@
         <v>32</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F12" t="s">
         <v>56</v>
@@ -4531,7 +4543,7 @@
         <v>32</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F14" t="s">
         <v>58</v>
@@ -7011,7 +7023,7 @@
         <v>31</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="F24" s="8" t="s">
         <v>69</v>
@@ -7507,7 +7519,7 @@
         <v>31</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F26" t="s">
         <v>72</v>
@@ -8995,7 +9007,7 @@
         <v>33</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="F32" t="s">
         <v>80</v>
@@ -9491,7 +9503,7 @@
         <v>33</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F34" t="s">
         <v>82</v>
@@ -11971,7 +11983,7 @@
         <v>28</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F44" t="s">
         <v>93</v>
@@ -12467,7 +12479,7 @@
         <v>28</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F46" t="s">
         <v>95</v>
@@ -13955,7 +13967,7 @@
         <v>32</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F52" t="s">
         <v>101</v>
@@ -14451,7 +14463,7 @@
         <v>32</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F54" t="s">
         <v>103</v>
@@ -16931,7 +16943,7 @@
         <v>31</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="F64" t="s">
         <v>110</v>
@@ -17427,7 +17439,7 @@
         <v>31</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F66" t="s">
         <v>112</v>
@@ -18188,14 +18200,14 @@
       <c r="J69" t="s">
         <v>31</v>
       </c>
-      <c r="K69" t="s">
-        <v>32</v>
-      </c>
-      <c r="L69">
-        <v>0</v>
-      </c>
-      <c r="M69" t="s">
-        <v>33</v>
+      <c r="K69" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L69" s="2">
+        <v>0</v>
+      </c>
+      <c r="M69" s="2">
+        <v>0</v>
       </c>
       <c r="N69" t="s">
         <v>34</v>
@@ -18915,7 +18927,7 @@
         <v>33</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="F72" t="s">
         <v>118</v>
@@ -19411,7 +19423,7 @@
         <v>33</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F74" t="s">
         <v>120</v>
@@ -20172,14 +20184,14 @@
       <c r="J77" t="s">
         <v>31</v>
       </c>
-      <c r="K77" t="s">
-        <v>32</v>
-      </c>
-      <c r="L77">
-        <v>0</v>
-      </c>
-      <c r="M77" t="s">
-        <v>33</v>
+      <c r="K77" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L77" s="2">
+        <v>0</v>
+      </c>
+      <c r="M77" s="2">
+        <v>0</v>
       </c>
       <c r="N77" t="s">
         <v>34</v>
@@ -21891,7 +21903,7 @@
         <v>28</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F84" t="s">
         <v>129</v>
@@ -22387,7 +22399,7 @@
         <v>28</v>
       </c>
       <c r="E86" s="6" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F86" t="s">
         <v>131</v>
@@ -23149,13 +23161,13 @@
         <v>31</v>
       </c>
       <c r="K89" s="2" t="s">
-        <v>135</v>
+        <v>32</v>
       </c>
       <c r="L89" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M89" s="2" t="s">
-        <v>136</v>
+        <v>33</v>
       </c>
       <c r="N89" s="2" t="s">
         <v>34</v>
@@ -23164,7 +23176,7 @@
         <v>35</v>
       </c>
       <c r="P89" s="2" t="s">
-        <v>137</v>
+        <v>36</v>
       </c>
       <c r="Q89">
         <v>0</v>
@@ -23251,7 +23263,7 @@
         <v>1</v>
       </c>
       <c r="AS89" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="AT89">
         <v>0</v>
@@ -23305,13 +23317,13 @@
         <v>0</v>
       </c>
       <c r="BK89" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="BL89">
         <v>1</v>
       </c>
       <c r="BM89" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="BN89">
         <v>0</v>
@@ -23382,7 +23394,7 @@
         <v>29</v>
       </c>
       <c r="F90" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G90">
         <v>120</v>
@@ -23630,7 +23642,7 @@
         <v>28</v>
       </c>
       <c r="F91" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G91">
         <v>120</v>
@@ -23875,10 +23887,10 @@
         <v>32</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F92" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G92">
         <v>120</v>
@@ -24126,7 +24138,7 @@
         <v>31</v>
       </c>
       <c r="F93" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G93">
         <v>120</v>
@@ -24371,10 +24383,10 @@
         <v>32</v>
       </c>
       <c r="E94" s="6" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F94" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G94">
         <v>120</v>
@@ -24622,7 +24634,7 @@
         <v>49</v>
       </c>
       <c r="F95" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G95">
         <v>120</v>
@@ -24870,7 +24882,7 @@
         <v>34</v>
       </c>
       <c r="F96" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G96">
         <v>120</v>
@@ -25133,13 +25145,13 @@
         <v>31</v>
       </c>
       <c r="K97" s="2" t="s">
-        <v>135</v>
+        <v>32</v>
       </c>
       <c r="L97" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M97" s="2" t="s">
-        <v>136</v>
+        <v>33</v>
       </c>
       <c r="N97" s="2" t="s">
         <v>34</v>
@@ -25148,7 +25160,7 @@
         <v>35</v>
       </c>
       <c r="P97" s="2" t="s">
-        <v>137</v>
+        <v>36</v>
       </c>
       <c r="Q97">
         <v>0</v>
@@ -25235,7 +25247,7 @@
         <v>1</v>
       </c>
       <c r="AS97" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="AT97">
         <v>0</v>
@@ -25289,13 +25301,13 @@
         <v>0</v>
       </c>
       <c r="BK97" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="BL97">
         <v>1</v>
       </c>
       <c r="BM97" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="BN97">
         <v>0</v>
@@ -25366,7 +25378,7 @@
         <v>29</v>
       </c>
       <c r="F98" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G98">
         <v>120</v>
@@ -25614,7 +25626,7 @@
         <v>28</v>
       </c>
       <c r="F99" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G99">
         <v>120</v>
@@ -25862,7 +25874,7 @@
         <v>31</v>
       </c>
       <c r="F100" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G100">
         <v>120</v>
@@ -26125,13 +26137,13 @@
         <v>31</v>
       </c>
       <c r="K101" s="2" t="s">
-        <v>135</v>
+        <v>32</v>
       </c>
       <c r="L101" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M101" s="2" t="s">
-        <v>136</v>
+        <v>33</v>
       </c>
       <c r="N101" s="2" t="s">
         <v>34</v>
@@ -26140,7 +26152,7 @@
         <v>35</v>
       </c>
       <c r="P101" s="2" t="s">
-        <v>137</v>
+        <v>36</v>
       </c>
       <c r="Q101">
         <v>0</v>
@@ -26227,7 +26239,7 @@
         <v>1</v>
       </c>
       <c r="AS101" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="AT101">
         <v>0</v>
@@ -26281,13 +26293,13 @@
         <v>0</v>
       </c>
       <c r="BK101" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="BL101">
         <v>1</v>
       </c>
       <c r="BM101" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="BN101">
         <v>0</v>
@@ -26358,7 +26370,7 @@
         <v>29</v>
       </c>
       <c r="F102" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G102">
         <v>120</v>
@@ -26606,7 +26618,7 @@
         <v>67</v>
       </c>
       <c r="F103" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G103">
         <v>120</v>
@@ -26851,10 +26863,10 @@
         <v>31</v>
       </c>
       <c r="E104" s="6" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="F104" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G104">
         <v>120</v>
@@ -27102,7 +27114,7 @@
         <v>70</v>
       </c>
       <c r="F105" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G105">
         <v>120</v>
@@ -27347,10 +27359,10 @@
         <v>31</v>
       </c>
       <c r="E106" s="6" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F106" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G106">
         <v>120</v>
@@ -27598,7 +27610,7 @@
         <v>73</v>
       </c>
       <c r="F107" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G107">
         <v>120</v>
@@ -27846,7 +27858,7 @@
         <v>75</v>
       </c>
       <c r="F108" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G108">
         <v>120</v>
@@ -28109,13 +28121,13 @@
         <v>31</v>
       </c>
       <c r="K109" s="2" t="s">
-        <v>135</v>
+        <v>32</v>
       </c>
       <c r="L109" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M109" s="2" t="s">
-        <v>136</v>
+        <v>33</v>
       </c>
       <c r="N109" s="2" t="s">
         <v>34</v>
@@ -28124,7 +28136,7 @@
         <v>35</v>
       </c>
       <c r="P109" s="2" t="s">
-        <v>137</v>
+        <v>36</v>
       </c>
       <c r="Q109">
         <v>0</v>
@@ -28211,7 +28223,7 @@
         <v>1</v>
       </c>
       <c r="AS109" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="AT109">
         <v>0</v>
@@ -28265,13 +28277,13 @@
         <v>0</v>
       </c>
       <c r="BK109" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="BL109">
         <v>1</v>
       </c>
       <c r="BM109" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="BN109">
         <v>0</v>
@@ -28342,7 +28354,7 @@
         <v>29</v>
       </c>
       <c r="F110" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G110">
         <v>120</v>
@@ -28590,7 +28602,7 @@
         <v>67</v>
       </c>
       <c r="F111" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G111">
         <v>120</v>
@@ -28835,10 +28847,10 @@
         <v>33</v>
       </c>
       <c r="E112" s="6" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="F112" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G112">
         <v>120</v>
@@ -29086,7 +29098,7 @@
         <v>70</v>
       </c>
       <c r="F113" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G113">
         <v>120</v>
@@ -29331,10 +29343,10 @@
         <v>33</v>
       </c>
       <c r="E114" s="6" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F114" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G114">
         <v>120</v>
@@ -29582,7 +29594,7 @@
         <v>73</v>
       </c>
       <c r="F115" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G115">
         <v>120</v>
@@ -29830,7 +29842,7 @@
         <v>75</v>
       </c>
       <c r="F116" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G116">
         <v>120</v>
@@ -30093,13 +30105,13 @@
         <v>31</v>
       </c>
       <c r="K117" s="2" t="s">
-        <v>135</v>
+        <v>32</v>
       </c>
       <c r="L117" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M117" s="2" t="s">
-        <v>136</v>
+        <v>33</v>
       </c>
       <c r="N117" s="2" t="s">
         <v>34</v>
@@ -30108,7 +30120,7 @@
         <v>35</v>
       </c>
       <c r="P117" s="2" t="s">
-        <v>137</v>
+        <v>36</v>
       </c>
       <c r="Q117">
         <v>0</v>
@@ -30195,7 +30207,7 @@
         <v>1</v>
       </c>
       <c r="AS117" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="AT117">
         <v>0</v>
@@ -30249,13 +30261,13 @@
         <v>0</v>
       </c>
       <c r="BK117" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="BL117">
         <v>1</v>
       </c>
       <c r="BM117" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="BN117">
         <v>0</v>
@@ -30326,7 +30338,7 @@
         <v>29</v>
       </c>
       <c r="F118" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G118">
         <v>120</v>
@@ -30574,7 +30586,7 @@
         <v>67</v>
       </c>
       <c r="F119" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G119">
         <v>120</v>
@@ -30822,7 +30834,7 @@
         <v>70</v>
       </c>
       <c r="F120" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G120">
         <v>120</v>
@@ -31085,13 +31097,13 @@
         <v>31</v>
       </c>
       <c r="K121" s="2" t="s">
-        <v>135</v>
+        <v>32</v>
       </c>
       <c r="L121" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M121" s="2" t="s">
-        <v>136</v>
+        <v>33</v>
       </c>
       <c r="N121" s="2" t="s">
         <v>34</v>
@@ -31100,7 +31112,7 @@
         <v>35</v>
       </c>
       <c r="P121" s="2" t="s">
-        <v>137</v>
+        <v>36</v>
       </c>
       <c r="Q121">
         <v>0</v>
@@ -31187,7 +31199,7 @@
         <v>1</v>
       </c>
       <c r="AS121" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="AT121">
         <v>0</v>
@@ -31241,13 +31253,13 @@
         <v>0</v>
       </c>
       <c r="BK121" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="BL121">
         <v>1</v>
       </c>
       <c r="BM121" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="BN121">
         <v>0</v>
@@ -31306,16 +31318,16 @@
         <v>45139</v>
       </c>
       <c r="C122" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E122" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="D122" s="2" t="s">
+      <c r="F122" t="s">
         <v>168</v>
-      </c>
-      <c r="E122" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="F122" t="s">
-        <v>170</v>
       </c>
       <c r="G122">
         <v>240</v>
@@ -31348,10 +31360,10 @@
         <v>36</v>
       </c>
       <c r="Q122" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="R122" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="S122" s="2">
         <v>0</v>
@@ -31554,16 +31566,16 @@
         <v>45139</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E123" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F123" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G123">
         <v>240</v>
@@ -31596,10 +31608,10 @@
         <v>36</v>
       </c>
       <c r="Q123" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="R123" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="S123" s="2">
         <v>0</v>
@@ -31802,16 +31814,16 @@
         <v>45139</v>
       </c>
       <c r="C124" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E124" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="D124" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E124" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="F124" t="s">
-        <v>176</v>
+      <c r="F124" s="8" t="s">
+        <v>255</v>
       </c>
       <c r="G124">
         <v>240</v>
@@ -31844,10 +31856,10 @@
         <v>36</v>
       </c>
       <c r="Q124" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="R124" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="S124" s="2">
         <v>0</v>
@@ -32050,16 +32062,16 @@
         <v>45139</v>
       </c>
       <c r="C125" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E125" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="D125" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E125" s="3" t="s">
-        <v>173</v>
-      </c>
       <c r="F125" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G125">
         <v>240</v>
@@ -32092,10 +32104,10 @@
         <v>36</v>
       </c>
       <c r="Q125" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="R125" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="S125" s="2">
         <v>0</v>
@@ -32298,16 +32310,16 @@
         <v>45139</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="E126" s="3" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="F126" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="G126">
         <v>240</v>
@@ -32340,10 +32352,10 @@
         <v>36</v>
       </c>
       <c r="Q126" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="R126" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="S126" s="2">
         <v>0</v>
@@ -32546,16 +32558,16 @@
         <v>45139</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>178</v>
+        <v>254</v>
       </c>
       <c r="E127" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="F127" t="s">
-        <v>180</v>
+        <v>171</v>
+      </c>
+      <c r="F127" s="8" t="s">
+        <v>256</v>
       </c>
       <c r="G127">
         <v>240</v>
@@ -32588,10 +32600,10 @@
         <v>36</v>
       </c>
       <c r="Q127" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="R127" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="S127" s="2">
         <v>0</v>
@@ -32794,16 +32806,16 @@
         <v>45139</v>
       </c>
       <c r="C128" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E128" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="D128" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="E128" s="3" t="s">
-        <v>169</v>
-      </c>
       <c r="F128" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="G128">
         <v>240</v>
@@ -32836,10 +32848,10 @@
         <v>36</v>
       </c>
       <c r="Q128" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="R128" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="S128" s="2">
         <v>0</v>
@@ -33042,16 +33054,16 @@
         <v>45139</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E129" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F129" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="G129">
         <v>240</v>
@@ -33084,10 +33096,10 @@
         <v>36</v>
       </c>
       <c r="Q129" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="R129" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="S129" s="2">
         <v>0</v>
@@ -33290,16 +33302,16 @@
         <v>45139</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F130" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="G130">
         <v>240</v>
@@ -33332,10 +33344,10 @@
         <v>36</v>
       </c>
       <c r="Q130" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="R130" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="S130" s="2">
         <v>0</v>
@@ -33538,16 +33550,16 @@
         <v>45139</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="E131" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F131" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="G131">
         <v>240</v>
@@ -33580,10 +33592,10 @@
         <v>36</v>
       </c>
       <c r="Q131" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="R131" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="S131" s="2">
         <v>0</v>
@@ -33786,16 +33798,16 @@
         <v>45139</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F132" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G132">
         <v>240</v>
@@ -33828,10 +33840,10 @@
         <v>36</v>
       </c>
       <c r="Q132" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="R132" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="S132" s="2">
         <v>0</v>
@@ -34034,16 +34046,16 @@
         <v>45139</v>
       </c>
       <c r="C133" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D133" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E133" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F133" t="s">
         <v>184</v>
-      </c>
-      <c r="D133" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E133" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="F133" t="s">
-        <v>188</v>
       </c>
       <c r="G133">
         <v>240</v>
@@ -34076,10 +34088,10 @@
         <v>36</v>
       </c>
       <c r="Q133" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="R133" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="S133" s="2">
         <v>0</v>
@@ -34282,16 +34294,16 @@
         <v>45139</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>178</v>
+        <v>253</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="F134" t="s">
-        <v>189</v>
+        <v>167</v>
+      </c>
+      <c r="F134" s="8" t="s">
+        <v>257</v>
       </c>
       <c r="G134">
         <v>240</v>
@@ -34324,10 +34336,10 @@
         <v>36</v>
       </c>
       <c r="Q134" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="R134" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="S134" s="2">
         <v>0</v>
@@ -34530,16 +34542,16 @@
         <v>45139</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="E135" s="3" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="F135" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="G135">
         <v>240</v>
@@ -34572,10 +34584,10 @@
         <v>36</v>
       </c>
       <c r="Q135" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="R135" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="S135" s="2">
         <v>0</v>
@@ -34778,16 +34790,16 @@
         <v>45139</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="E136" s="3" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="F136" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="G136">
         <v>240</v>
@@ -34820,10 +34832,10 @@
         <v>36</v>
       </c>
       <c r="Q136" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="R136" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="S136" s="2">
         <v>0</v>
@@ -35026,16 +35038,16 @@
         <v>45139</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>181</v>
+        <v>254</v>
       </c>
       <c r="E137" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="F137" t="s">
-        <v>192</v>
+        <v>171</v>
+      </c>
+      <c r="F137" s="8" t="s">
+        <v>258</v>
       </c>
       <c r="G137">
         <v>240</v>
@@ -35068,10 +35080,10 @@
         <v>36</v>
       </c>
       <c r="Q137" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="R137" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="S137" s="2">
         <v>0</v>
@@ -35274,16 +35286,16 @@
         <v>45139</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
       <c r="E138" s="3" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="F138" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="G138">
         <v>240</v>
@@ -35300,8 +35312,8 @@
       <c r="K138" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L138" s="2" t="s">
-        <v>135</v>
+      <c r="L138" s="2">
+        <v>0</v>
       </c>
       <c r="M138" s="2" t="s">
         <v>31</v>
@@ -35316,10 +35328,10 @@
         <v>36</v>
       </c>
       <c r="Q138" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="R138" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="S138" s="2">
         <v>0</v>
@@ -35522,16 +35534,16 @@
         <v>45139</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
       <c r="E139" s="3" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="F139" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="G139">
         <v>240</v>
@@ -35548,8 +35560,8 @@
       <c r="K139" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L139" s="2" t="s">
-        <v>135</v>
+      <c r="L139" s="2">
+        <v>0</v>
       </c>
       <c r="M139" s="2" t="s">
         <v>31</v>
@@ -35564,10 +35576,10 @@
         <v>36</v>
       </c>
       <c r="Q139" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="R139" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="S139" s="2">
         <v>0</v>
@@ -35770,16 +35782,16 @@
         <v>45139</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>49</v>
+        <v>179</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="F140" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="G140">
         <v>240</v>
@@ -35796,8 +35808,8 @@
       <c r="K140" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L140" s="2" t="s">
-        <v>135</v>
+      <c r="L140" s="2">
+        <v>0</v>
       </c>
       <c r="M140" s="2" t="s">
         <v>31</v>
@@ -35812,10 +35824,10 @@
         <v>36</v>
       </c>
       <c r="Q140" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="R140" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="S140" s="2">
         <v>0</v>
@@ -36018,16 +36030,16 @@
         <v>45139</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>49</v>
+        <v>179</v>
       </c>
       <c r="E141" s="3" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="F141" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="G141">
         <v>240</v>
@@ -36044,8 +36056,8 @@
       <c r="K141" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L141" s="2" t="s">
-        <v>135</v>
+      <c r="L141" s="2">
+        <v>0</v>
       </c>
       <c r="M141" s="2" t="s">
         <v>31</v>
@@ -36060,10 +36072,10 @@
         <v>36</v>
       </c>
       <c r="Q141" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="R141" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="S141" s="2">
         <v>0</v>
@@ -36266,16 +36278,16 @@
         <v>45139</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="E142" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F142" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="G142">
         <v>240</v>
@@ -36308,10 +36320,10 @@
         <v>36</v>
       </c>
       <c r="Q142" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="R142" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="S142" s="2">
         <v>0</v>
@@ -36514,16 +36526,16 @@
         <v>45139</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="E143" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F143" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="G143">
         <v>240</v>
@@ -36556,10 +36568,10 @@
         <v>36</v>
       </c>
       <c r="Q143" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="R143" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="S143" s="2">
         <v>0</v>
@@ -36762,16 +36774,16 @@
         <v>45139</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>203</v>
+        <v>49</v>
       </c>
       <c r="E144" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F144" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="G144">
         <v>240</v>
@@ -36804,10 +36816,10 @@
         <v>36</v>
       </c>
       <c r="Q144" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="R144" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="S144" s="2">
         <v>0</v>
@@ -37010,16 +37022,16 @@
         <v>45139</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>203</v>
+        <v>49</v>
       </c>
       <c r="E145" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F145" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="G145">
         <v>240</v>
@@ -37052,10 +37064,10 @@
         <v>36</v>
       </c>
       <c r="Q145" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="R145" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="S145" s="2">
         <v>0</v>
@@ -37258,16 +37270,16 @@
         <v>45139</v>
       </c>
       <c r="C146" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E146" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F146" t="s">
         <v>199</v>
-      </c>
-      <c r="D146" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="E146" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="F146" t="s">
-        <v>207</v>
       </c>
       <c r="G146">
         <v>240</v>
@@ -37300,10 +37312,10 @@
         <v>36</v>
       </c>
       <c r="Q146" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="R146" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="S146" s="2">
         <v>0</v>
@@ -37506,16 +37518,16 @@
         <v>45139</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="E147" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F147" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="G147">
         <v>240</v>
@@ -37548,10 +37560,10 @@
         <v>36</v>
       </c>
       <c r="Q147" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="R147" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="S147" s="2">
         <v>0</v>
@@ -37754,16 +37766,16 @@
         <v>45139</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="E148" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F148" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="G148">
         <v>240</v>
@@ -37796,10 +37808,10 @@
         <v>36</v>
       </c>
       <c r="Q148" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="R148" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="S148" s="2">
         <v>0</v>
@@ -38002,16 +38014,16 @@
         <v>45139</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="E149" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F149" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="G149">
         <v>240</v>
@@ -38044,10 +38056,10 @@
         <v>36</v>
       </c>
       <c r="Q149" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="R149" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="S149" s="2">
         <v>0</v>
@@ -38250,16 +38262,16 @@
         <v>45139</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="D150" t="s">
-        <v>194</v>
-      </c>
-      <c r="E150" s="10" t="s">
-        <v>173</v>
+        <v>197</v>
+      </c>
+      <c r="D150" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="E150" s="3" t="s">
+        <v>171</v>
       </c>
       <c r="F150" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="G150">
         <v>240</v>
@@ -38292,10 +38304,10 @@
         <v>36</v>
       </c>
       <c r="Q150" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="R150" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="S150" s="2">
         <v>0</v>
@@ -38498,16 +38510,16 @@
         <v>45139</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="D151" t="s">
-        <v>49</v>
-      </c>
-      <c r="E151" s="10" t="s">
-        <v>169</v>
+        <v>197</v>
+      </c>
+      <c r="D151" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="E151" s="3" t="s">
+        <v>167</v>
       </c>
       <c r="F151" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="G151">
         <v>240</v>
@@ -38540,10 +38552,10 @@
         <v>36</v>
       </c>
       <c r="Q151" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="R151" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="S151" s="2">
         <v>0</v>
@@ -38746,13 +38758,19 @@
         <v>45139</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>214</v>
+        <v>197</v>
+      </c>
+      <c r="D152" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E152" s="3" t="s">
+        <v>171</v>
       </c>
       <c r="F152" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="G152">
-        <v>210</v>
+        <v>240</v>
       </c>
       <c r="H152">
         <v>180</v>
@@ -38763,29 +38781,29 @@
       <c r="J152" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K152" s="2">
-        <v>0</v>
-      </c>
-      <c r="L152" s="2">
-        <v>0</v>
-      </c>
-      <c r="M152" s="2">
-        <v>0</v>
-      </c>
-      <c r="N152" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="O152" s="2">
-        <v>0</v>
-      </c>
-      <c r="P152" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q152" s="2">
-        <v>0</v>
-      </c>
-      <c r="R152" s="2">
-        <v>0</v>
+      <c r="K152" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L152" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="M152" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="N152" s="2">
+        <v>0</v>
+      </c>
+      <c r="O152" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P152" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q152" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="R152" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="S152" s="2">
         <v>0</v>
@@ -38812,16 +38830,16 @@
         <v>0</v>
       </c>
       <c r="AA152">
-        <v>210</v>
+        <v>240</v>
       </c>
       <c r="AB152">
         <v>180</v>
       </c>
-      <c r="AC152" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD152" s="2" t="s">
-        <v>31</v>
+      <c r="AC152">
+        <v>0</v>
+      </c>
+      <c r="AD152">
+        <v>0</v>
       </c>
       <c r="AE152">
         <v>0</v>
@@ -38832,8 +38850,8 @@
       <c r="AG152">
         <v>0</v>
       </c>
-      <c r="AH152" s="2" t="s">
-        <v>216</v>
+      <c r="AH152">
+        <v>0</v>
       </c>
       <c r="AI152">
         <v>0</v>
@@ -38988,16 +39006,22 @@
         <v>45139</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>217</v>
+        <v>197</v>
+      </c>
+      <c r="D153" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E153" s="3" t="s">
+        <v>167</v>
       </c>
       <c r="F153" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="G153">
-        <v>190</v>
+        <v>240</v>
       </c>
       <c r="H153">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="I153" s="2" t="s">
         <v>28</v>
@@ -39009,13 +39033,13 @@
         <v>32</v>
       </c>
       <c r="L153" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="M153" s="2">
-        <v>0</v>
-      </c>
-      <c r="N153" s="2" t="s">
-        <v>34</v>
+        <v>135</v>
+      </c>
+      <c r="M153" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="N153" s="2">
+        <v>0</v>
       </c>
       <c r="O153" s="2" t="s">
         <v>35</v>
@@ -39023,11 +39047,11 @@
       <c r="P153" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="Q153">
-        <v>0</v>
-      </c>
-      <c r="R153">
-        <v>0</v>
+      <c r="Q153" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="R153" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="S153" s="2">
         <v>0</v>
@@ -39054,10 +39078,10 @@
         <v>0</v>
       </c>
       <c r="AA153">
-        <v>190</v>
+        <v>240</v>
       </c>
       <c r="AB153">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="AC153">
         <v>0</v>
@@ -39230,16 +39254,22 @@
         <v>45139</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>219</v>
+        <v>210</v>
+      </c>
+      <c r="D154" t="s">
+        <v>192</v>
+      </c>
+      <c r="E154" s="10" t="s">
+        <v>171</v>
       </c>
       <c r="F154" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="G154">
-        <v>220</v>
+        <v>240</v>
       </c>
       <c r="H154">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="I154" s="2" t="s">
         <v>28</v>
@@ -39253,11 +39283,11 @@
       <c r="L154" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="M154" s="2">
-        <v>0</v>
-      </c>
-      <c r="N154" s="2" t="s">
-        <v>34</v>
+      <c r="M154" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="N154" s="2">
+        <v>0</v>
       </c>
       <c r="O154" s="2" t="s">
         <v>35</v>
@@ -39266,10 +39296,10 @@
         <v>36</v>
       </c>
       <c r="Q154" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="R154" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="S154" s="2">
         <v>0</v>
@@ -39296,10 +39326,10 @@
         <v>0</v>
       </c>
       <c r="AA154">
-        <v>220</v>
+        <v>240</v>
       </c>
       <c r="AB154">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="AC154">
         <v>0</v>
@@ -39472,16 +39502,22 @@
         <v>45139</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="F155" s="8" t="s">
-        <v>249</v>
+        <v>210</v>
+      </c>
+      <c r="D155" t="s">
+        <v>49</v>
+      </c>
+      <c r="E155" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="F155" t="s">
+        <v>211</v>
       </c>
       <c r="G155">
-        <v>170</v>
+        <v>240</v>
       </c>
       <c r="H155">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="I155" s="2" t="s">
         <v>28</v>
@@ -39495,11 +39531,11 @@
       <c r="L155" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="M155" s="2">
-        <v>0</v>
-      </c>
-      <c r="N155" s="2" t="s">
-        <v>34</v>
+      <c r="M155" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="N155" s="2">
+        <v>0</v>
       </c>
       <c r="O155" s="2" t="s">
         <v>35</v>
@@ -39508,13 +39544,13 @@
         <v>36</v>
       </c>
       <c r="Q155" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="R155" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="S155" s="2" t="s">
-        <v>222</v>
+        <v>170</v>
+      </c>
+      <c r="S155" s="2">
+        <v>0</v>
       </c>
       <c r="T155" s="2">
         <v>0</v>
@@ -39538,10 +39574,10 @@
         <v>0</v>
       </c>
       <c r="AA155">
-        <v>170</v>
+        <v>240</v>
       </c>
       <c r="AB155">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="AC155">
         <v>0</v>
@@ -39714,16 +39750,16 @@
         <v>45139</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="F156" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="G156">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="H156">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="I156" s="2" t="s">
         <v>28</v>
@@ -39731,11 +39767,11 @@
       <c r="J156" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K156" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="L156" s="2" t="s">
-        <v>135</v>
+      <c r="K156" s="2">
+        <v>0</v>
+      </c>
+      <c r="L156" s="2">
+        <v>0</v>
       </c>
       <c r="M156" s="2">
         <v>0</v>
@@ -39743,17 +39779,17 @@
       <c r="N156" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="O156" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="P156" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q156" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="R156" s="2" t="s">
-        <v>172</v>
+      <c r="O156" s="2">
+        <v>0</v>
+      </c>
+      <c r="P156" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q156" s="2">
+        <v>0</v>
+      </c>
+      <c r="R156" s="2">
+        <v>0</v>
       </c>
       <c r="S156" s="2">
         <v>0</v>
@@ -39780,16 +39816,16 @@
         <v>0</v>
       </c>
       <c r="AA156">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="AB156">
-        <v>190</v>
-      </c>
-      <c r="AC156">
-        <v>0</v>
-      </c>
-      <c r="AD156">
-        <v>0</v>
+        <v>180</v>
+      </c>
+      <c r="AC156" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD156" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="AE156">
         <v>0</v>
@@ -39800,8 +39836,8 @@
       <c r="AG156">
         <v>0</v>
       </c>
-      <c r="AH156">
-        <v>0</v>
+      <c r="AH156" s="2" t="s">
+        <v>214</v>
       </c>
       <c r="AI156">
         <v>0</v>
@@ -39956,16 +39992,16 @@
         <v>45139</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="F157" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="G157">
-        <v>220</v>
+        <v>190</v>
       </c>
       <c r="H157">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="I157" s="2" t="s">
         <v>28</v>
@@ -39973,11 +40009,11 @@
       <c r="J157" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K157">
-        <v>0</v>
-      </c>
-      <c r="L157">
-        <v>0</v>
+      <c r="K157" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L157" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="M157" s="2">
         <v>0</v>
@@ -39985,11 +40021,11 @@
       <c r="N157" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="O157">
-        <v>0</v>
-      </c>
-      <c r="P157">
-        <v>0</v>
+      <c r="O157" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P157" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="Q157">
         <v>0</v>
@@ -40022,10 +40058,10 @@
         <v>0</v>
       </c>
       <c r="AA157">
-        <v>220</v>
+        <v>190</v>
       </c>
       <c r="AB157">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="AC157">
         <v>0</v>
@@ -40198,19 +40234,16 @@
         <v>45139</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="D158" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="F158" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="G158">
         <v>220</v>
       </c>
       <c r="H158">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="I158" s="2" t="s">
         <v>28</v>
@@ -40218,11 +40251,11 @@
       <c r="J158" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K158" s="2">
-        <v>0</v>
-      </c>
-      <c r="L158" s="2">
-        <v>0</v>
+      <c r="K158" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L158" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="M158" s="2">
         <v>0</v>
@@ -40230,17 +40263,17 @@
       <c r="N158" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="O158" s="2">
-        <v>0</v>
-      </c>
-      <c r="P158" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q158" s="2">
-        <v>0</v>
-      </c>
-      <c r="R158" s="2">
-        <v>0</v>
+      <c r="O158" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P158" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q158" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="R158" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="S158" s="2">
         <v>0</v>
@@ -40270,7 +40303,7 @@
         <v>220</v>
       </c>
       <c r="AB158">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="AC158">
         <v>0</v>
@@ -40443,19 +40476,16 @@
         <v>45139</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="D159" t="s">
-        <v>230</v>
-      </c>
-      <c r="F159" t="s">
-        <v>231</v>
+        <v>219</v>
+      </c>
+      <c r="F159" s="8" t="s">
+        <v>247</v>
       </c>
       <c r="G159">
-        <v>220</v>
+        <v>170</v>
       </c>
       <c r="H159">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="I159" s="2" t="s">
         <v>28</v>
@@ -40463,11 +40493,11 @@
       <c r="J159" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K159">
-        <v>0</v>
-      </c>
-      <c r="L159">
-        <v>0</v>
+      <c r="K159" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L159" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="M159" s="2">
         <v>0</v>
@@ -40475,20 +40505,20 @@
       <c r="N159" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="O159">
-        <v>0</v>
-      </c>
-      <c r="P159">
-        <v>0</v>
-      </c>
-      <c r="Q159">
-        <v>0</v>
-      </c>
-      <c r="R159">
-        <v>0</v>
-      </c>
-      <c r="S159" s="2">
-        <v>0</v>
+      <c r="O159" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P159" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q159" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="R159" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="S159" s="2" t="s">
+        <v>220</v>
       </c>
       <c r="T159" s="2">
         <v>0</v>
@@ -40512,10 +40542,10 @@
         <v>0</v>
       </c>
       <c r="AA159">
-        <v>220</v>
+        <v>170</v>
       </c>
       <c r="AB159">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="AC159">
         <v>0</v>
@@ -40688,16 +40718,16 @@
         <v>45139</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="F160" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="G160">
-        <v>240</v>
+        <v>190</v>
       </c>
       <c r="H160">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="I160" s="2" t="s">
         <v>28</v>
@@ -40705,29 +40735,29 @@
       <c r="J160" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K160" s="2">
-        <v>0</v>
-      </c>
-      <c r="L160" s="2">
-        <v>0</v>
+      <c r="K160" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L160" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="M160" s="2">
         <v>0</v>
       </c>
       <c r="N160" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="O160" s="2">
-        <v>0</v>
-      </c>
-      <c r="P160" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q160" s="2">
-        <v>0</v>
-      </c>
-      <c r="R160" s="2">
-        <v>0</v>
+        <v>34</v>
+      </c>
+      <c r="O160" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P160" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q160" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="R160" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="S160" s="2">
         <v>0</v>
@@ -40754,10 +40784,10 @@
         <v>0</v>
       </c>
       <c r="AA160">
-        <v>240</v>
+        <v>190</v>
       </c>
       <c r="AB160">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="AC160">
         <v>0</v>
@@ -40930,13 +40960,13 @@
         <v>45139</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="F161" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="G161">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="H161">
         <v>180</v>
@@ -40947,8 +40977,8 @@
       <c r="J161" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K161" s="2" t="s">
-        <v>91</v>
+      <c r="K161">
+        <v>0</v>
       </c>
       <c r="L161">
         <v>0</v>
@@ -40957,7 +40987,7 @@
         <v>0</v>
       </c>
       <c r="N161" s="2" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="O161">
         <v>0</v>
@@ -40996,16 +41026,16 @@
         <v>0</v>
       </c>
       <c r="AA161">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="AB161">
         <v>180</v>
       </c>
-      <c r="AC161" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD161" s="2" t="s">
-        <v>31</v>
+      <c r="AC161">
+        <v>0</v>
+      </c>
+      <c r="AD161">
+        <v>0</v>
       </c>
       <c r="AE161">
         <v>0</v>
@@ -41016,8 +41046,8 @@
       <c r="AG161">
         <v>0</v>
       </c>
-      <c r="AH161" s="2" t="s">
-        <v>49</v>
+      <c r="AH161">
+        <v>0</v>
       </c>
       <c r="AI161">
         <v>0</v>
@@ -41172,16 +41202,16 @@
         <v>45139</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="D162" s="2" t="s">
-        <v>49</v>
+        <v>225</v>
+      </c>
+      <c r="D162" t="s">
+        <v>226</v>
       </c>
       <c r="F162" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="G162">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="H162">
         <v>180</v>
@@ -41192,10 +41222,10 @@
       <c r="J162" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K162">
-        <v>0</v>
-      </c>
-      <c r="L162">
+      <c r="K162" s="2">
+        <v>0</v>
+      </c>
+      <c r="L162" s="2">
         <v>0</v>
       </c>
       <c r="M162" s="2">
@@ -41204,16 +41234,16 @@
       <c r="N162" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="O162">
-        <v>0</v>
-      </c>
-      <c r="P162">
-        <v>0</v>
-      </c>
-      <c r="Q162">
-        <v>0</v>
-      </c>
-      <c r="R162">
+      <c r="O162" s="2">
+        <v>0</v>
+      </c>
+      <c r="P162" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q162" s="2">
+        <v>0</v>
+      </c>
+      <c r="R162" s="2">
         <v>0</v>
       </c>
       <c r="S162" s="2">
@@ -41241,7 +41271,7 @@
         <v>0</v>
       </c>
       <c r="AA162">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="AB162">
         <v>180</v>
@@ -41417,16 +41447,16 @@
         <v>45139</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="D163" s="2" t="s">
-        <v>194</v>
+        <v>225</v>
+      </c>
+      <c r="D163" t="s">
+        <v>228</v>
       </c>
       <c r="F163" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
       <c r="G163">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="H163">
         <v>180</v>
@@ -41437,10 +41467,10 @@
       <c r="J163" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K163" s="2">
-        <v>0</v>
-      </c>
-      <c r="L163" s="2">
+      <c r="K163">
+        <v>0</v>
+      </c>
+      <c r="L163">
         <v>0</v>
       </c>
       <c r="M163" s="2">
@@ -41449,16 +41479,16 @@
       <c r="N163" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="O163" s="2">
-        <v>0</v>
-      </c>
-      <c r="P163" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q163" s="2">
-        <v>0</v>
-      </c>
-      <c r="R163" s="2">
+      <c r="O163">
+        <v>0</v>
+      </c>
+      <c r="P163">
+        <v>0</v>
+      </c>
+      <c r="Q163">
+        <v>0</v>
+      </c>
+      <c r="R163">
         <v>0</v>
       </c>
       <c r="S163" s="2">
@@ -41486,7 +41516,7 @@
         <v>0</v>
       </c>
       <c r="AA163">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="AB163">
         <v>180</v>
@@ -41662,19 +41692,16 @@
         <v>45139</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="D164" s="2" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="F164" t="s">
+        <v>231</v>
+      </c>
+      <c r="G164">
         <v>240</v>
       </c>
-      <c r="G164">
-        <v>250</v>
-      </c>
       <c r="H164">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="I164" s="2" t="s">
         <v>28</v>
@@ -41682,41 +41709,41 @@
       <c r="J164" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K164" s="2" t="s">
-        <v>91</v>
+      <c r="K164" s="2">
+        <v>0</v>
       </c>
       <c r="L164" s="2">
         <v>0</v>
       </c>
-      <c r="M164" s="2" t="s">
-        <v>34</v>
+      <c r="M164" s="2">
+        <v>0</v>
       </c>
       <c r="N164" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="O164" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="P164" s="2" t="s">
-        <v>36</v>
+        <v>49</v>
+      </c>
+      <c r="O164" s="2">
+        <v>0</v>
+      </c>
+      <c r="P164" s="2">
+        <v>0</v>
       </c>
       <c r="Q164" s="2">
         <v>0</v>
       </c>
-      <c r="R164">
-        <v>0</v>
-      </c>
-      <c r="S164" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="T164" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="U164" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="V164" s="2" t="s">
-        <v>40</v>
+      <c r="R164" s="2">
+        <v>0</v>
+      </c>
+      <c r="S164" s="2">
+        <v>0</v>
+      </c>
+      <c r="T164" s="2">
+        <v>0</v>
+      </c>
+      <c r="U164" s="2">
+        <v>0</v>
+      </c>
+      <c r="V164" s="2">
+        <v>0</v>
       </c>
       <c r="W164" s="2" t="s">
         <v>41</v>
@@ -41731,10 +41758,10 @@
         <v>0</v>
       </c>
       <c r="AA164">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="AB164">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="AC164">
         <v>0</v>
@@ -41907,19 +41934,16 @@
         <v>45139</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="D165" t="s">
-        <v>221</v>
+        <v>232</v>
       </c>
       <c r="F165" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="G165">
         <v>250</v>
       </c>
       <c r="H165">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="I165" s="2" t="s">
         <v>28</v>
@@ -41930,38 +41954,38 @@
       <c r="K165" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="L165" s="2">
-        <v>0</v>
-      </c>
-      <c r="M165" s="2" t="s">
-        <v>34</v>
+      <c r="L165">
+        <v>0</v>
+      </c>
+      <c r="M165" s="2">
+        <v>0</v>
       </c>
       <c r="N165" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="O165" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="P165" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q165" s="2">
-        <v>0</v>
-      </c>
-      <c r="R165" s="2">
-        <v>0</v>
-      </c>
-      <c r="S165" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="T165" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="U165" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="V165" s="2" t="s">
-        <v>40</v>
+        <v>49</v>
+      </c>
+      <c r="O165">
+        <v>0</v>
+      </c>
+      <c r="P165">
+        <v>0</v>
+      </c>
+      <c r="Q165">
+        <v>0</v>
+      </c>
+      <c r="R165">
+        <v>0</v>
+      </c>
+      <c r="S165" s="2">
+        <v>0</v>
+      </c>
+      <c r="T165" s="2">
+        <v>0</v>
+      </c>
+      <c r="U165" s="2">
+        <v>0</v>
+      </c>
+      <c r="V165" s="2">
+        <v>0</v>
       </c>
       <c r="W165" s="2" t="s">
         <v>41</v>
@@ -41979,13 +42003,13 @@
         <v>250</v>
       </c>
       <c r="AB165">
-        <v>90</v>
-      </c>
-      <c r="AC165">
-        <v>0</v>
-      </c>
-      <c r="AD165">
-        <v>0</v>
+        <v>180</v>
+      </c>
+      <c r="AC165" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD165" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="AE165">
         <v>0</v>
@@ -41996,8 +42020,8 @@
       <c r="AG165">
         <v>0</v>
       </c>
-      <c r="AH165">
-        <v>0</v>
+      <c r="AH165" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="AI165">
         <v>0</v>
@@ -42152,19 +42176,19 @@
         <v>45139</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="D166" t="s">
-        <v>242</v>
+        <v>234</v>
+      </c>
+      <c r="D166" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="F166" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="G166">
         <v>250</v>
       </c>
       <c r="H166">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="I166" s="2" t="s">
         <v>28</v>
@@ -42172,23 +42196,23 @@
       <c r="J166" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K166" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="L166" s="2">
-        <v>0</v>
-      </c>
-      <c r="M166" s="2" t="s">
+      <c r="K166">
+        <v>0</v>
+      </c>
+      <c r="L166">
+        <v>0</v>
+      </c>
+      <c r="M166" s="2">
+        <v>0</v>
+      </c>
+      <c r="N166" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="N166" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="O166" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="P166" s="2" t="s">
-        <v>36</v>
+      <c r="O166">
+        <v>0</v>
+      </c>
+      <c r="P166">
+        <v>0</v>
       </c>
       <c r="Q166">
         <v>0</v>
@@ -42196,17 +42220,17 @@
       <c r="R166">
         <v>0</v>
       </c>
-      <c r="S166" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="T166" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="U166" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="V166" s="2" t="s">
-        <v>40</v>
+      <c r="S166" s="2">
+        <v>0</v>
+      </c>
+      <c r="T166" s="2">
+        <v>0</v>
+      </c>
+      <c r="U166" s="2">
+        <v>0</v>
+      </c>
+      <c r="V166" s="2">
+        <v>0</v>
       </c>
       <c r="W166" s="2" t="s">
         <v>41</v>
@@ -42224,7 +42248,7 @@
         <v>250</v>
       </c>
       <c r="AB166">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="AC166">
         <v>0</v>
@@ -42397,16 +42421,19 @@
         <v>45139</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>243</v>
+        <v>234</v>
+      </c>
+      <c r="D167" s="2" t="s">
+        <v>192</v>
       </c>
       <c r="F167" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="G167">
-        <v>170</v>
+        <v>250</v>
       </c>
       <c r="H167">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="I167" s="2" t="s">
         <v>28</v>
@@ -42424,7 +42451,7 @@
         <v>0</v>
       </c>
       <c r="N167" s="2" t="s">
-        <v>216</v>
+        <v>34</v>
       </c>
       <c r="O167" s="2">
         <v>0</v>
@@ -42463,10 +42490,10 @@
         <v>0</v>
       </c>
       <c r="AA167">
-        <v>170</v>
+        <v>250</v>
       </c>
       <c r="AB167">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="AC167">
         <v>0</v>
@@ -42638,59 +42665,62 @@
       <c r="B168" s="5">
         <v>45139</v>
       </c>
-      <c r="C168" t="s">
-        <v>244</v>
+      <c r="C168" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D168" s="2" t="s">
+        <v>237</v>
       </c>
       <c r="F168" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="G168">
-        <v>170</v>
+        <v>250</v>
       </c>
       <c r="H168">
-        <v>170</v>
-      </c>
-      <c r="I168">
-        <v>0</v>
-      </c>
-      <c r="J168">
-        <v>0</v>
-      </c>
-      <c r="K168">
-        <v>0</v>
-      </c>
-      <c r="L168">
-        <v>0</v>
-      </c>
-      <c r="M168">
-        <v>0</v>
-      </c>
-      <c r="N168">
-        <v>0</v>
-      </c>
-      <c r="O168">
-        <v>0</v>
-      </c>
-      <c r="P168">
-        <v>0</v>
-      </c>
-      <c r="Q168">
+        <v>90</v>
+      </c>
+      <c r="I168" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J168" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K168" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L168" s="2">
+        <v>0</v>
+      </c>
+      <c r="M168" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N168" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="O168" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P168" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q168" s="2">
         <v>0</v>
       </c>
       <c r="R168">
         <v>0</v>
       </c>
-      <c r="S168">
-        <v>0</v>
-      </c>
-      <c r="T168">
-        <v>0</v>
-      </c>
-      <c r="U168">
-        <v>0</v>
-      </c>
-      <c r="V168">
-        <v>0</v>
+      <c r="S168" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T168" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U168" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="V168" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="W168" s="2" t="s">
         <v>41</v>
@@ -42705,10 +42735,10 @@
         <v>0</v>
       </c>
       <c r="AA168">
-        <v>170</v>
+        <v>250</v>
       </c>
       <c r="AB168">
-        <v>170</v>
+        <v>90</v>
       </c>
       <c r="AC168">
         <v>0</v>
@@ -42880,59 +42910,62 @@
       <c r="B169" s="5">
         <v>45139</v>
       </c>
-      <c r="C169" t="s">
-        <v>245</v>
+      <c r="C169" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D169" t="s">
+        <v>219</v>
       </c>
       <c r="F169" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="G169">
-        <v>170</v>
+        <v>250</v>
       </c>
       <c r="H169">
-        <v>170</v>
-      </c>
-      <c r="I169">
-        <v>0</v>
-      </c>
-      <c r="J169">
-        <v>0</v>
-      </c>
-      <c r="K169">
-        <v>0</v>
-      </c>
-      <c r="L169">
-        <v>0</v>
-      </c>
-      <c r="M169">
-        <v>0</v>
-      </c>
-      <c r="N169">
-        <v>0</v>
-      </c>
-      <c r="O169">
-        <v>0</v>
-      </c>
-      <c r="P169">
-        <v>0</v>
-      </c>
-      <c r="Q169">
-        <v>0</v>
-      </c>
-      <c r="R169">
-        <v>0</v>
-      </c>
-      <c r="S169">
-        <v>0</v>
-      </c>
-      <c r="T169">
-        <v>0</v>
-      </c>
-      <c r="U169">
-        <v>0</v>
-      </c>
-      <c r="V169">
-        <v>0</v>
+        <v>90</v>
+      </c>
+      <c r="I169" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J169" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K169" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L169" s="2">
+        <v>0</v>
+      </c>
+      <c r="M169" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N169" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="O169" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P169" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q169" s="2">
+        <v>0</v>
+      </c>
+      <c r="R169" s="2">
+        <v>0</v>
+      </c>
+      <c r="S169" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T169" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U169" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="V169" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="W169" s="2" t="s">
         <v>41</v>
@@ -42947,10 +42980,10 @@
         <v>0</v>
       </c>
       <c r="AA169">
-        <v>170</v>
+        <v>250</v>
       </c>
       <c r="AB169">
-        <v>170</v>
+        <v>90</v>
       </c>
       <c r="AC169">
         <v>0</v>
@@ -43112,18 +43145,993 @@
         <v>0</v>
       </c>
       <c r="CD169">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:82" x14ac:dyDescent="0.2">
+      <c r="A170" s="4">
+        <v>168</v>
+      </c>
+      <c r="B170" s="5">
+        <v>45139</v>
+      </c>
+      <c r="C170" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D170" t="s">
+        <v>240</v>
+      </c>
+      <c r="F170" t="s">
+        <v>245</v>
+      </c>
+      <c r="G170">
+        <v>250</v>
+      </c>
+      <c r="H170">
+        <v>90</v>
+      </c>
+      <c r="I170" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J170" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K170" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L170" s="2">
+        <v>0</v>
+      </c>
+      <c r="M170" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N170" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="O170" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P170" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q170">
+        <v>0</v>
+      </c>
+      <c r="R170">
+        <v>0</v>
+      </c>
+      <c r="S170" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T170" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U170" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="V170" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="W170" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="X170">
+        <v>0</v>
+      </c>
+      <c r="Y170" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z170" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA170">
+        <v>250</v>
+      </c>
+      <c r="AB170">
+        <v>90</v>
+      </c>
+      <c r="AC170">
+        <v>0</v>
+      </c>
+      <c r="AD170">
+        <v>0</v>
+      </c>
+      <c r="AE170">
+        <v>0</v>
+      </c>
+      <c r="AF170">
+        <v>0</v>
+      </c>
+      <c r="AG170">
+        <v>0</v>
+      </c>
+      <c r="AH170">
+        <v>0</v>
+      </c>
+      <c r="AI170">
+        <v>0</v>
+      </c>
+      <c r="AJ170">
+        <v>0</v>
+      </c>
+      <c r="AK170">
+        <v>0</v>
+      </c>
+      <c r="AL170">
+        <v>0</v>
+      </c>
+      <c r="AM170">
+        <v>0</v>
+      </c>
+      <c r="AN170">
+        <v>0</v>
+      </c>
+      <c r="AO170">
+        <v>0</v>
+      </c>
+      <c r="AP170">
+        <v>0</v>
+      </c>
+      <c r="AQ170" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AR170">
+        <v>0</v>
+      </c>
+      <c r="AS170" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AT170">
+        <v>0</v>
+      </c>
+      <c r="AU170">
+        <v>0</v>
+      </c>
+      <c r="AV170">
+        <v>0</v>
+      </c>
+      <c r="AW170">
+        <v>0</v>
+      </c>
+      <c r="AX170">
+        <v>0</v>
+      </c>
+      <c r="AY170">
+        <v>0</v>
+      </c>
+      <c r="AZ170">
+        <v>0</v>
+      </c>
+      <c r="BA170">
+        <v>0</v>
+      </c>
+      <c r="BB170">
+        <v>0</v>
+      </c>
+      <c r="BC170">
+        <v>0</v>
+      </c>
+      <c r="BD170">
+        <v>0</v>
+      </c>
+      <c r="BE170">
+        <v>0</v>
+      </c>
+      <c r="BF170">
+        <v>0</v>
+      </c>
+      <c r="BG170">
+        <v>0</v>
+      </c>
+      <c r="BH170">
+        <v>0</v>
+      </c>
+      <c r="BI170">
+        <v>0</v>
+      </c>
+      <c r="BJ170">
+        <v>0</v>
+      </c>
+      <c r="BK170" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="BL170">
+        <v>0</v>
+      </c>
+      <c r="BM170" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="BN170">
+        <v>0</v>
+      </c>
+      <c r="BO170">
+        <v>0</v>
+      </c>
+      <c r="BP170">
+        <v>0</v>
+      </c>
+      <c r="BQ170">
+        <v>0</v>
+      </c>
+      <c r="BR170">
+        <v>0</v>
+      </c>
+      <c r="BS170">
+        <v>0</v>
+      </c>
+      <c r="BT170">
+        <v>0</v>
+      </c>
+      <c r="BU170">
+        <v>0</v>
+      </c>
+      <c r="BV170">
+        <v>0</v>
+      </c>
+      <c r="BW170">
+        <v>0</v>
+      </c>
+      <c r="BX170">
+        <v>0</v>
+      </c>
+      <c r="BY170">
+        <v>0</v>
+      </c>
+      <c r="BZ170">
+        <v>0</v>
+      </c>
+      <c r="CA170">
+        <v>0</v>
+      </c>
+      <c r="CB170">
+        <v>0</v>
+      </c>
+      <c r="CC170">
+        <v>0</v>
+      </c>
+      <c r="CD170">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:82" x14ac:dyDescent="0.2">
+      <c r="A171" s="4">
+        <v>169</v>
+      </c>
+      <c r="B171" s="5">
+        <v>45139</v>
+      </c>
+      <c r="C171" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="F171" t="s">
+        <v>246</v>
+      </c>
+      <c r="G171">
+        <v>170</v>
+      </c>
+      <c r="H171">
+        <v>170</v>
+      </c>
+      <c r="I171" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J171" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K171" s="2">
+        <v>0</v>
+      </c>
+      <c r="L171" s="2">
+        <v>0</v>
+      </c>
+      <c r="M171" s="2">
+        <v>0</v>
+      </c>
+      <c r="N171" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="O171" s="2">
+        <v>0</v>
+      </c>
+      <c r="P171" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q171" s="2">
+        <v>0</v>
+      </c>
+      <c r="R171" s="2">
+        <v>0</v>
+      </c>
+      <c r="S171" s="2">
+        <v>0</v>
+      </c>
+      <c r="T171" s="2">
+        <v>0</v>
+      </c>
+      <c r="U171" s="2">
+        <v>0</v>
+      </c>
+      <c r="V171" s="2">
+        <v>0</v>
+      </c>
+      <c r="W171" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="X171">
+        <v>0</v>
+      </c>
+      <c r="Y171" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z171" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA171">
+        <v>170</v>
+      </c>
+      <c r="AB171">
+        <v>170</v>
+      </c>
+      <c r="AC171">
+        <v>0</v>
+      </c>
+      <c r="AD171">
+        <v>0</v>
+      </c>
+      <c r="AE171">
+        <v>0</v>
+      </c>
+      <c r="AF171">
+        <v>0</v>
+      </c>
+      <c r="AG171">
+        <v>0</v>
+      </c>
+      <c r="AH171">
+        <v>0</v>
+      </c>
+      <c r="AI171">
+        <v>0</v>
+      </c>
+      <c r="AJ171">
+        <v>0</v>
+      </c>
+      <c r="AK171">
+        <v>0</v>
+      </c>
+      <c r="AL171">
+        <v>0</v>
+      </c>
+      <c r="AM171">
+        <v>0</v>
+      </c>
+      <c r="AN171">
+        <v>0</v>
+      </c>
+      <c r="AO171">
+        <v>0</v>
+      </c>
+      <c r="AP171">
+        <v>0</v>
+      </c>
+      <c r="AQ171" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AR171">
+        <v>0</v>
+      </c>
+      <c r="AS171" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AT171">
+        <v>0</v>
+      </c>
+      <c r="AU171">
+        <v>0</v>
+      </c>
+      <c r="AV171">
+        <v>0</v>
+      </c>
+      <c r="AW171">
+        <v>0</v>
+      </c>
+      <c r="AX171">
+        <v>0</v>
+      </c>
+      <c r="AY171">
+        <v>0</v>
+      </c>
+      <c r="AZ171">
+        <v>0</v>
+      </c>
+      <c r="BA171">
+        <v>0</v>
+      </c>
+      <c r="BB171">
+        <v>0</v>
+      </c>
+      <c r="BC171">
+        <v>0</v>
+      </c>
+      <c r="BD171">
+        <v>0</v>
+      </c>
+      <c r="BE171">
+        <v>0</v>
+      </c>
+      <c r="BF171">
+        <v>0</v>
+      </c>
+      <c r="BG171">
+        <v>0</v>
+      </c>
+      <c r="BH171">
+        <v>0</v>
+      </c>
+      <c r="BI171">
+        <v>0</v>
+      </c>
+      <c r="BJ171">
+        <v>0</v>
+      </c>
+      <c r="BK171" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="BL171">
+        <v>0</v>
+      </c>
+      <c r="BM171" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="BN171">
+        <v>0</v>
+      </c>
+      <c r="BO171">
+        <v>0</v>
+      </c>
+      <c r="BP171">
+        <v>0</v>
+      </c>
+      <c r="BQ171">
+        <v>0</v>
+      </c>
+      <c r="BR171">
+        <v>0</v>
+      </c>
+      <c r="BS171">
+        <v>0</v>
+      </c>
+      <c r="BT171">
+        <v>0</v>
+      </c>
+      <c r="BU171">
+        <v>0</v>
+      </c>
+      <c r="BV171">
+        <v>0</v>
+      </c>
+      <c r="BW171">
+        <v>0</v>
+      </c>
+      <c r="BX171">
+        <v>0</v>
+      </c>
+      <c r="BY171">
+        <v>0</v>
+      </c>
+      <c r="BZ171">
+        <v>0</v>
+      </c>
+      <c r="CA171">
+        <v>0</v>
+      </c>
+      <c r="CB171">
+        <v>0</v>
+      </c>
+      <c r="CC171">
+        <v>0</v>
+      </c>
+      <c r="CD171">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:82" x14ac:dyDescent="0.2">
+      <c r="A172" s="4">
+        <v>170</v>
+      </c>
+      <c r="B172" s="5">
+        <v>45139</v>
+      </c>
+      <c r="C172" t="s">
+        <v>242</v>
+      </c>
+      <c r="F172" t="s">
+        <v>246</v>
+      </c>
+      <c r="G172">
+        <v>170</v>
+      </c>
+      <c r="H172">
+        <v>170</v>
+      </c>
+      <c r="I172">
+        <v>0</v>
+      </c>
+      <c r="J172">
+        <v>0</v>
+      </c>
+      <c r="K172">
+        <v>0</v>
+      </c>
+      <c r="L172">
+        <v>0</v>
+      </c>
+      <c r="M172">
+        <v>0</v>
+      </c>
+      <c r="N172">
+        <v>0</v>
+      </c>
+      <c r="O172">
+        <v>0</v>
+      </c>
+      <c r="P172">
+        <v>0</v>
+      </c>
+      <c r="Q172">
+        <v>0</v>
+      </c>
+      <c r="R172">
+        <v>0</v>
+      </c>
+      <c r="S172">
+        <v>0</v>
+      </c>
+      <c r="T172">
+        <v>0</v>
+      </c>
+      <c r="U172">
+        <v>0</v>
+      </c>
+      <c r="V172">
+        <v>0</v>
+      </c>
+      <c r="W172" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="X172">
+        <v>0</v>
+      </c>
+      <c r="Y172" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z172" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA172">
+        <v>170</v>
+      </c>
+      <c r="AB172">
+        <v>170</v>
+      </c>
+      <c r="AC172">
+        <v>0</v>
+      </c>
+      <c r="AD172">
+        <v>0</v>
+      </c>
+      <c r="AE172">
+        <v>0</v>
+      </c>
+      <c r="AF172">
+        <v>0</v>
+      </c>
+      <c r="AG172">
+        <v>0</v>
+      </c>
+      <c r="AH172">
+        <v>0</v>
+      </c>
+      <c r="AI172">
+        <v>0</v>
+      </c>
+      <c r="AJ172">
+        <v>0</v>
+      </c>
+      <c r="AK172">
+        <v>0</v>
+      </c>
+      <c r="AL172">
+        <v>0</v>
+      </c>
+      <c r="AM172">
+        <v>0</v>
+      </c>
+      <c r="AN172">
+        <v>0</v>
+      </c>
+      <c r="AO172">
+        <v>0</v>
+      </c>
+      <c r="AP172">
+        <v>0</v>
+      </c>
+      <c r="AQ172" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AR172">
+        <v>0</v>
+      </c>
+      <c r="AS172" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AT172">
+        <v>0</v>
+      </c>
+      <c r="AU172">
+        <v>0</v>
+      </c>
+      <c r="AV172">
+        <v>0</v>
+      </c>
+      <c r="AW172">
+        <v>0</v>
+      </c>
+      <c r="AX172">
+        <v>0</v>
+      </c>
+      <c r="AY172">
+        <v>0</v>
+      </c>
+      <c r="AZ172">
+        <v>0</v>
+      </c>
+      <c r="BA172">
+        <v>0</v>
+      </c>
+      <c r="BB172">
+        <v>0</v>
+      </c>
+      <c r="BC172">
+        <v>0</v>
+      </c>
+      <c r="BD172">
+        <v>0</v>
+      </c>
+      <c r="BE172">
+        <v>0</v>
+      </c>
+      <c r="BF172">
+        <v>0</v>
+      </c>
+      <c r="BG172">
+        <v>0</v>
+      </c>
+      <c r="BH172">
+        <v>0</v>
+      </c>
+      <c r="BI172">
+        <v>0</v>
+      </c>
+      <c r="BJ172">
+        <v>0</v>
+      </c>
+      <c r="BK172" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="BL172">
+        <v>0</v>
+      </c>
+      <c r="BM172" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="BN172">
+        <v>0</v>
+      </c>
+      <c r="BO172">
+        <v>0</v>
+      </c>
+      <c r="BP172">
+        <v>0</v>
+      </c>
+      <c r="BQ172">
+        <v>0</v>
+      </c>
+      <c r="BR172">
+        <v>0</v>
+      </c>
+      <c r="BS172">
+        <v>0</v>
+      </c>
+      <c r="BT172">
+        <v>0</v>
+      </c>
+      <c r="BU172">
+        <v>0</v>
+      </c>
+      <c r="BV172">
+        <v>0</v>
+      </c>
+      <c r="BW172">
+        <v>0</v>
+      </c>
+      <c r="BX172">
+        <v>0</v>
+      </c>
+      <c r="BY172">
+        <v>0</v>
+      </c>
+      <c r="BZ172">
+        <v>0</v>
+      </c>
+      <c r="CA172">
+        <v>0</v>
+      </c>
+      <c r="CB172">
+        <v>0</v>
+      </c>
+      <c r="CC172">
+        <v>0</v>
+      </c>
+      <c r="CD172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:82" x14ac:dyDescent="0.2">
+      <c r="A173" s="4">
+        <v>171</v>
+      </c>
+      <c r="B173" s="5">
+        <v>45139</v>
+      </c>
+      <c r="C173" t="s">
+        <v>243</v>
+      </c>
+      <c r="F173" t="s">
+        <v>246</v>
+      </c>
+      <c r="G173">
+        <v>170</v>
+      </c>
+      <c r="H173">
+        <v>170</v>
+      </c>
+      <c r="I173">
+        <v>0</v>
+      </c>
+      <c r="J173">
+        <v>0</v>
+      </c>
+      <c r="K173">
+        <v>0</v>
+      </c>
+      <c r="L173">
+        <v>0</v>
+      </c>
+      <c r="M173">
+        <v>0</v>
+      </c>
+      <c r="N173">
+        <v>0</v>
+      </c>
+      <c r="O173">
+        <v>0</v>
+      </c>
+      <c r="P173">
+        <v>0</v>
+      </c>
+      <c r="Q173">
+        <v>0</v>
+      </c>
+      <c r="R173">
+        <v>0</v>
+      </c>
+      <c r="S173">
+        <v>0</v>
+      </c>
+      <c r="T173">
+        <v>0</v>
+      </c>
+      <c r="U173">
+        <v>0</v>
+      </c>
+      <c r="V173">
+        <v>0</v>
+      </c>
+      <c r="W173" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="X173">
+        <v>0</v>
+      </c>
+      <c r="Y173" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z173" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA173">
+        <v>170</v>
+      </c>
+      <c r="AB173">
+        <v>170</v>
+      </c>
+      <c r="AC173">
+        <v>0</v>
+      </c>
+      <c r="AD173">
+        <v>0</v>
+      </c>
+      <c r="AE173">
+        <v>0</v>
+      </c>
+      <c r="AF173">
+        <v>0</v>
+      </c>
+      <c r="AG173">
+        <v>0</v>
+      </c>
+      <c r="AH173">
+        <v>0</v>
+      </c>
+      <c r="AI173">
+        <v>0</v>
+      </c>
+      <c r="AJ173">
+        <v>0</v>
+      </c>
+      <c r="AK173">
+        <v>0</v>
+      </c>
+      <c r="AL173">
+        <v>0</v>
+      </c>
+      <c r="AM173">
+        <v>0</v>
+      </c>
+      <c r="AN173">
+        <v>0</v>
+      </c>
+      <c r="AO173">
+        <v>0</v>
+      </c>
+      <c r="AP173">
+        <v>0</v>
+      </c>
+      <c r="AQ173" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AR173">
+        <v>0</v>
+      </c>
+      <c r="AS173" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AT173">
+        <v>0</v>
+      </c>
+      <c r="AU173">
+        <v>0</v>
+      </c>
+      <c r="AV173">
+        <v>0</v>
+      </c>
+      <c r="AW173">
+        <v>0</v>
+      </c>
+      <c r="AX173">
+        <v>0</v>
+      </c>
+      <c r="AY173">
+        <v>0</v>
+      </c>
+      <c r="AZ173">
+        <v>0</v>
+      </c>
+      <c r="BA173">
+        <v>0</v>
+      </c>
+      <c r="BB173">
+        <v>0</v>
+      </c>
+      <c r="BC173">
+        <v>0</v>
+      </c>
+      <c r="BD173">
+        <v>0</v>
+      </c>
+      <c r="BE173">
+        <v>0</v>
+      </c>
+      <c r="BF173">
+        <v>0</v>
+      </c>
+      <c r="BG173">
+        <v>0</v>
+      </c>
+      <c r="BH173">
+        <v>0</v>
+      </c>
+      <c r="BI173">
+        <v>0</v>
+      </c>
+      <c r="BJ173">
+        <v>0</v>
+      </c>
+      <c r="BK173" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="BL173">
+        <v>0</v>
+      </c>
+      <c r="BM173" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="BN173">
+        <v>0</v>
+      </c>
+      <c r="BO173">
+        <v>0</v>
+      </c>
+      <c r="BP173">
+        <v>0</v>
+      </c>
+      <c r="BQ173">
+        <v>0</v>
+      </c>
+      <c r="BR173">
+        <v>0</v>
+      </c>
+      <c r="BS173">
+        <v>0</v>
+      </c>
+      <c r="BT173">
+        <v>0</v>
+      </c>
+      <c r="BU173">
+        <v>0</v>
+      </c>
+      <c r="BV173">
+        <v>0</v>
+      </c>
+      <c r="BW173">
+        <v>0</v>
+      </c>
+      <c r="BX173">
+        <v>0</v>
+      </c>
+      <c r="BY173">
+        <v>0</v>
+      </c>
+      <c r="BZ173">
+        <v>0</v>
+      </c>
+      <c r="CA173">
+        <v>0</v>
+      </c>
+      <c r="CB173">
+        <v>0</v>
+      </c>
+      <c r="CC173">
+        <v>0</v>
+      </c>
+      <c r="CD173">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F155" r:id="rId1" xr:uid="{2EBCD065-C0A9-4D0D-974B-0ABD6971AC2C}"/>
+    <hyperlink ref="F159" r:id="rId1" xr:uid="{2EBCD065-C0A9-4D0D-974B-0ABD6971AC2C}"/>
     <hyperlink ref="F39" r:id="rId2" xr:uid="{93300645-12C2-4500-B601-CC5EA36EE083}"/>
     <hyperlink ref="F10" r:id="rId3" xr:uid="{8AA8E1B1-DE7C-4056-A2A2-6DACCBCF8316}"/>
     <hyperlink ref="F24" r:id="rId4" xr:uid="{44C2B535-F755-42A7-87CF-80F1D4EDA9E5}"/>
+    <hyperlink ref="F124" r:id="rId5" xr:uid="{A44C4CDF-411A-4EE3-AFD9-E549429DC73C}"/>
+    <hyperlink ref="F127" r:id="rId6" xr:uid="{9891D545-5BE7-4162-9F82-99F187AE80DF}"/>
+    <hyperlink ref="F134" r:id="rId7" xr:uid="{CF10C34F-1DC6-4E6A-818B-A1D47625BFD4}"/>
+    <hyperlink ref="F137" r:id="rId8" xr:uid="{C4BFBD49-530E-449E-B29C-6619C4A43276}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="57" fitToHeight="0" orientation="landscape" r:id="rId5"/>
+  <pageSetup paperSize="9" scale="57" fitToHeight="0" orientation="landscape" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
mise à jour nom plans
</commit_message>
<xml_diff>
--- a/Remote/Commun/dist_liens.xlsx
+++ b/Remote/Commun/dist_liens.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Mickaël\Documents\GitHub\ductaironline\ductaironline\Remote\Commun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6524014D-98A2-4C70-97BF-CBC8AA41C36D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9832AB3-B516-4D64-BF33-201A42DDF319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5430" yWindow="1995" windowWidth="21600" windowHeight="11295" xr2:uid="{10E80606-BDFD-48EA-859F-8B282D217FD1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{10E80606-BDFD-48EA-859F-8B282D217FD1}"/>
   </bookViews>
   <sheets>
     <sheet name="dist_liens" sheetId="1" r:id="rId1"/>
@@ -179,13 +179,7 @@
     <t>https://ductair.github.io/ductaironline/Drawings/TCC/FACE/A/A.jpg</t>
   </si>
   <si>
-    <t>https://ductair.github.io/ductaironline/Drawings/TCC/FACE/A/A'.jpg</t>
-  </si>
-  <si>
     <t>https://ductair.github.io/ductaironline/Drawings/TCC/FACE/A/B.jpg</t>
-  </si>
-  <si>
-    <t>https://ductair.github.io/ductaironline/Drawings/TCC/FACE/A/B'.jpg</t>
   </si>
   <si>
     <t>C</t>
@@ -209,13 +203,7 @@
     <t>https://ductair.github.io/ductaironline/Drawings/TCC/FACE/A1/A.jpg</t>
   </si>
   <si>
-    <t>https://ductair.github.io/ductaironline/Drawings/TCC/FACE/A1/A'.jpg</t>
-  </si>
-  <si>
     <t>https://ductair.github.io/ductaironline/Drawings/TCC/FACE/A1/B.jpg</t>
-  </si>
-  <si>
-    <t>https://ductair.github.io/ductaironline/Drawings/TCC/FACE/A1/B'.jpg</t>
   </si>
   <si>
     <t>https://ductair.github.io/ductaironline/Drawings/TCC/FACE/A1/C.jpg</t>
@@ -248,16 +236,10 @@
     <t>https://ductair.github.io/ductaironline/Drawings/TCC/COTE/B/1.jpg</t>
   </si>
   <si>
-    <t>https://ductair.github.io/ductaironline/Drawings/TCC/COTE/B/1'.jpg</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
     <t>https://ductair.github.io/ductaironline/Drawings/TCC/COTE/B/2.jpg</t>
-  </si>
-  <si>
-    <t>https://ductair.github.io/ductaironline/Drawings/TCC/COTE/B/2'.jpg</t>
   </si>
   <si>
     <t>3</t>
@@ -281,13 +263,7 @@
     <t>https://ductair.github.io/ductaironline/Drawings/TCC/COTE/B1/1.jpg</t>
   </si>
   <si>
-    <t>https://ductair.github.io/ductaironline/Drawings/TCC/COTE/B1/1'.jpg</t>
-  </si>
-  <si>
     <t>https://ductair.github.io/ductaironline/Drawings/TCC/COTE/B1/2.jpg</t>
-  </si>
-  <si>
-    <t>https://ductair.github.io/ductaironline/Drawings/TCC/COTE/B1/2'.jpg</t>
   </si>
   <si>
     <t>https://ductair.github.io/ductaironline/Drawings/TCC/COTE/B1/3.jpg</t>
@@ -320,13 +296,7 @@
     <t>https://ductair.github.io/ductaironline/Drawings/TRC/FACE/A/A.jpg</t>
   </si>
   <si>
-    <t>https://ductair.github.io/ductaironline/Drawings/TRC/FACE/A/A'.jpg</t>
-  </si>
-  <si>
     <t>https://ductair.github.io/ductaironline/Drawings/TRC/FACE/A/B.jpg</t>
-  </si>
-  <si>
-    <t>https://ductair.github.io/ductaironline/Drawings/TRC/FACE/A/B'.jpg</t>
   </si>
   <si>
     <t>https://ductair.github.io/ductaironline/Drawings/TRC/FACE/A/C.jpg</t>
@@ -344,13 +314,7 @@
     <t>https://ductair.github.io/ductaironline/Drawings/TRC/FACE/Ø/A.jpg</t>
   </si>
   <si>
-    <t>https://ductair.github.io/ductaironline/Drawings/TRC/FACE/Ø/A'.jpg</t>
-  </si>
-  <si>
     <t>https://ductair.github.io/ductaironline/Drawings/TRC/FACE/Ø/B.jpg</t>
-  </si>
-  <si>
-    <t>https://ductair.github.io/ductaironline/Drawings/TRC/FACE/Ø/B'.jpg</t>
   </si>
   <si>
     <t>https://ductair.github.io/ductaironline/Drawings/TRC/FACE/Ø/C.jpg</t>
@@ -371,13 +335,7 @@
     <t>https://ductair.github.io/ductaironline/Drawings/TRC/COTE/B/1.jpg</t>
   </si>
   <si>
-    <t>https://ductair.github.io/ductaironline/Drawings/TRC/COTE/B/1'.jpg</t>
-  </si>
-  <si>
     <t>https://ductair.github.io/ductaironline/Drawings/TRC/COTE/B/2.jpg</t>
-  </si>
-  <si>
-    <t>https://ductair.github.io/ductaironline/Drawings/TRC/COTE/B/2'.jpg</t>
   </si>
   <si>
     <t>https://ductair.github.io/ductaironline/Drawings/TRC/COTE/B/3.jpg</t>
@@ -395,13 +353,7 @@
     <t>https://ductair.github.io/ductaironline/Drawings/TRC/COTE/Ø/1.jpg</t>
   </si>
   <si>
-    <t>https://ductair.github.io/ductaironline/Drawings/TRC/COTE/Ø/1'.jpg</t>
-  </si>
-  <si>
     <t>https://ductair.github.io/ductaironline/Drawings/TRC/COTE/Ø/2.jpg</t>
-  </si>
-  <si>
-    <t>https://ductair.github.io/ductaironline/Drawings/TRC/COTE/Ø/2'.jpg</t>
   </si>
   <si>
     <t>https://ductair.github.io/ductaironline/Drawings/TRC/COTE/Ø/3.jpg</t>
@@ -428,13 +380,7 @@
     <t>https://ductair.github.io/ductaironline/Drawings/PLR/FACE/A/A.jpg</t>
   </si>
   <si>
-    <t>https://ductair.github.io/ductaironline/Drawings/PLR/FACE/A/A'.jpg</t>
-  </si>
-  <si>
     <t>https://ductair.github.io/ductaironline/Drawings/PLR/FACE/A/B.jpg</t>
-  </si>
-  <si>
-    <t>https://ductair.github.io/ductaironline/Drawings/PLR/FACE/A/B'.jpg</t>
   </si>
   <si>
     <t>https://ductair.github.io/ductaironline/Drawings/PLR/FACE/A/C.jpg</t>
@@ -461,13 +407,7 @@
     <t>https://ductair.github.io/ductaironline/Drawings/PLR/FACE/A1/A.jpg</t>
   </si>
   <si>
-    <t>https://ductair.github.io/ductaironline/Drawings/PLR/FACE/A1/A'.jpg</t>
-  </si>
-  <si>
     <t>https://ductair.github.io/ductaironline/Drawings/PLR/FACE/A1/B.jpg</t>
-  </si>
-  <si>
-    <t>https://ductair.github.io/ductaironline/Drawings/PLR/FACE/A1/B'.jpg</t>
   </si>
   <si>
     <t>https://ductair.github.io/ductaironline/Drawings/PLR/FACE/A1/C.jpg</t>
@@ -491,13 +431,7 @@
     <t>https://ductair.github.io/ductaironline/Drawings/PLR/COTE/B/1.jpg</t>
   </si>
   <si>
-    <t>https://ductair.github.io/ductaironline/Drawings/PLR/COTE/B/1'.jpg</t>
-  </si>
-  <si>
     <t>https://ductair.github.io/ductaironline/Drawings/PLR/COTE/B/2.jpg</t>
-  </si>
-  <si>
-    <t>https://ductair.github.io/ductaironline/Drawings/PLR/COTE/B/2'.jpg</t>
   </si>
   <si>
     <t>https://ductair.github.io/ductaironline/Drawings/PLR/COTE/B/3.jpg</t>
@@ -512,13 +446,7 @@
     <t>https://ductair.github.io/ductaironline/Drawings/PLR/COTE/B1/1.jpg</t>
   </si>
   <si>
-    <t>https://ductair.github.io/ductaironline/Drawings/PLR/COTE/B1/1'.jpg</t>
-  </si>
-  <si>
     <t>https://ductair.github.io/ductaironline/Drawings/PLR/COTE/B1/2.jpg</t>
-  </si>
-  <si>
-    <t>https://ductair.github.io/ductaironline/Drawings/PLR/COTE/B1/2'.jpg</t>
   </si>
   <si>
     <t>https://ductair.github.io/ductaironline/Drawings/PLR/COTE/B1/3.jpg</t>
@@ -816,6 +744,78 @@
   </si>
   <si>
     <t>https://ductair.github.io/ductaironline/Drawings/C/C45/RAYON/C45carre.jpg</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Drawings/TCC/FACE/A/Ap.jpg</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Drawings/TCC/FACE/A/Bp.jpg</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Drawings/TCC/FACE/A1/Ap.jpg</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Drawings/TCC/FACE/A1/Bp.jpg</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Drawings/TCC/COTE/B/1p.jpg</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Drawings/TCC/COTE/B/2p.jpg</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Drawings/TCC/COTE/B1/1p.jpg</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Drawings/TCC/COTE/B1/2p.jpg</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Drawings/TRC/FACE/A/Ap.jpg</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Drawings/TRC/FACE/A/Bp.jpg</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Drawings/TRC/FACE/Ø/Ap.jpg</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Drawings/TRC/FACE/Ø/Bp.jpg</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Drawings/TRC/COTE/B/1p.jpg</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Drawings/TRC/COTE/B/2p.jpg</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Drawings/TRC/COTE/Ø/1p.jpg</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Drawings/TRC/COTE/Ø/2p.jpg</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Drawings/PLR/FACE/A/Ap.jpg</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Drawings/PLR/FACE/A/Bp.jpg</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Drawings/PLR/FACE/A1/Ap.jpg</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Drawings/PLR/FACE/A1/Bp.jpg</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Drawings/PLR/COTE/B/1p.jpg</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Drawings/PLR/COTE/B/2p.jpg</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Drawings/PLR/COTE/B1/1p.jpg</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Drawings/PLR/COTE/B1/2p.jpg</t>
   </si>
 </sst>
 </file>
@@ -1227,8 +1227,8 @@
   <dimension ref="A1:CD173"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E136" sqref="E136"/>
+      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F114" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2063,10 +2063,10 @@
         <v>28</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="F4" t="s">
-        <v>46</v>
+        <v>225</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>235</v>
       </c>
       <c r="G4">
         <v>120</v>
@@ -2314,7 +2314,7 @@
         <v>31</v>
       </c>
       <c r="F5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G5">
         <v>120</v>
@@ -2559,10 +2559,10 @@
         <v>28</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>250</v>
+        <v>226</v>
       </c>
       <c r="F6" t="s">
-        <v>48</v>
+        <v>236</v>
       </c>
       <c r="G6">
         <v>120</v>
@@ -2807,10 +2807,10 @@
         <v>28</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G7">
         <v>120</v>
@@ -3058,7 +3058,7 @@
         <v>34</v>
       </c>
       <c r="F8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G8">
         <v>120</v>
@@ -3303,10 +3303,10 @@
         <v>28</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G9">
         <v>120</v>
@@ -3554,7 +3554,7 @@
         <v>29</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>248</v>
+        <v>224</v>
       </c>
       <c r="G10">
         <v>120</v>
@@ -3802,7 +3802,7 @@
         <v>28</v>
       </c>
       <c r="F11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G11">
         <v>120</v>
@@ -4047,10 +4047,10 @@
         <v>32</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>249</v>
+        <v>225</v>
       </c>
       <c r="F12" t="s">
-        <v>56</v>
+        <v>237</v>
       </c>
       <c r="G12">
         <v>120</v>
@@ -4298,7 +4298,7 @@
         <v>31</v>
       </c>
       <c r="F13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G13">
         <v>120</v>
@@ -4543,10 +4543,10 @@
         <v>32</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>250</v>
+        <v>226</v>
       </c>
       <c r="F14" t="s">
-        <v>58</v>
+        <v>238</v>
       </c>
       <c r="G14">
         <v>120</v>
@@ -4791,10 +4791,10 @@
         <v>32</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="G15">
         <v>120</v>
@@ -5042,7 +5042,7 @@
         <v>34</v>
       </c>
       <c r="F16" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G16">
         <v>120</v>
@@ -5287,10 +5287,10 @@
         <v>32</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G17">
         <v>120</v>
@@ -5532,13 +5532,13 @@
         <v>27</v>
       </c>
       <c r="D18" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>29</v>
       </c>
       <c r="F18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G18">
         <v>120</v>
@@ -5780,13 +5780,13 @@
         <v>27</v>
       </c>
       <c r="D19" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>28</v>
       </c>
       <c r="F19" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G19">
         <v>120</v>
@@ -6028,13 +6028,13 @@
         <v>27</v>
       </c>
       <c r="D20" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>31</v>
       </c>
       <c r="F20" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G20">
         <v>120</v>
@@ -6276,13 +6276,13 @@
         <v>27</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G21">
         <v>120</v>
@@ -6530,7 +6530,7 @@
         <v>29</v>
       </c>
       <c r="F22" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G22">
         <v>120</v>
@@ -6775,10 +6775,10 @@
         <v>31</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F23" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G23">
         <v>120</v>
@@ -7023,10 +7023,10 @@
         <v>31</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>69</v>
+        <v>239</v>
       </c>
       <c r="G24">
         <v>120</v>
@@ -7271,10 +7271,10 @@
         <v>31</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F25" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G25">
         <v>120</v>
@@ -7519,10 +7519,10 @@
         <v>31</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>252</v>
+        <v>228</v>
       </c>
       <c r="F26" t="s">
-        <v>72</v>
+        <v>240</v>
       </c>
       <c r="G26">
         <v>120</v>
@@ -7767,10 +7767,10 @@
         <v>31</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F27" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G27">
         <v>120</v>
@@ -8015,10 +8015,10 @@
         <v>31</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F28" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="G28">
         <v>120</v>
@@ -8263,10 +8263,10 @@
         <v>31</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F29" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G29">
         <v>120</v>
@@ -8514,7 +8514,7 @@
         <v>29</v>
       </c>
       <c r="F30" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="G30">
         <v>120</v>
@@ -8759,10 +8759,10 @@
         <v>33</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F31" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G31">
         <v>120</v>
@@ -9007,10 +9007,10 @@
         <v>33</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="F32" t="s">
-        <v>80</v>
+        <v>241</v>
       </c>
       <c r="G32">
         <v>120</v>
@@ -9255,10 +9255,10 @@
         <v>33</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F33" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="G33">
         <v>120</v>
@@ -9503,10 +9503,10 @@
         <v>33</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>252</v>
+        <v>228</v>
       </c>
       <c r="F34" t="s">
-        <v>82</v>
+        <v>242</v>
       </c>
       <c r="G34">
         <v>120</v>
@@ -9751,10 +9751,10 @@
         <v>33</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F35" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="G35">
         <v>120</v>
@@ -9999,10 +9999,10 @@
         <v>33</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F36" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="G36">
         <v>120</v>
@@ -10247,10 +10247,10 @@
         <v>33</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F37" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G37">
         <v>120</v>
@@ -10492,13 +10492,13 @@
         <v>27</v>
       </c>
       <c r="D38" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>29</v>
       </c>
       <c r="F38" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G38">
         <v>120</v>
@@ -10740,13 +10740,13 @@
         <v>27</v>
       </c>
       <c r="D39" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="G39">
         <v>120</v>
@@ -10988,13 +10988,13 @@
         <v>27</v>
       </c>
       <c r="D40" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F40" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="G40">
         <v>120</v>
@@ -11236,13 +11236,13 @@
         <v>27</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F41" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G41">
         <v>120</v>
@@ -11481,7 +11481,7 @@
         <v>45139</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D42" t="s">
         <v>28</v>
@@ -11490,7 +11490,7 @@
         <v>29</v>
       </c>
       <c r="F42" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="G42">
         <v>120</v>
@@ -11505,7 +11505,7 @@
         <v>31</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L42" s="2">
         <v>0</v>
@@ -11729,7 +11729,7 @@
         <v>45139</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D43" t="s">
         <v>28</v>
@@ -11738,7 +11738,7 @@
         <v>28</v>
       </c>
       <c r="F43" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="G43">
         <v>120</v>
@@ -11753,7 +11753,7 @@
         <v>31</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L43" s="2">
         <v>0</v>
@@ -11977,16 +11977,16 @@
         <v>45139</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D44" t="s">
         <v>28</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>249</v>
+        <v>225</v>
       </c>
       <c r="F44" t="s">
-        <v>93</v>
+        <v>243</v>
       </c>
       <c r="G44">
         <v>120</v>
@@ -12001,7 +12001,7 @@
         <v>31</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L44" s="2">
         <v>0</v>
@@ -12225,7 +12225,7 @@
         <v>45139</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D45" t="s">
         <v>28</v>
@@ -12234,7 +12234,7 @@
         <v>31</v>
       </c>
       <c r="F45" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G45">
         <v>120</v>
@@ -12249,7 +12249,7 @@
         <v>31</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L45" s="2">
         <v>0</v>
@@ -12473,16 +12473,16 @@
         <v>45139</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D46" t="s">
         <v>28</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>250</v>
+        <v>226</v>
       </c>
       <c r="F46" t="s">
-        <v>95</v>
+        <v>244</v>
       </c>
       <c r="G46">
         <v>120</v>
@@ -12497,7 +12497,7 @@
         <v>31</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L46" s="2">
         <v>0</v>
@@ -12721,16 +12721,16 @@
         <v>45139</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D47" t="s">
         <v>28</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F47" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="G47">
         <v>120</v>
@@ -12745,7 +12745,7 @@
         <v>31</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L47" s="2">
         <v>0</v>
@@ -12969,7 +12969,7 @@
         <v>45139</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D48" t="s">
         <v>28</v>
@@ -12978,7 +12978,7 @@
         <v>34</v>
       </c>
       <c r="F48" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="G48">
         <v>120</v>
@@ -12993,7 +12993,7 @@
         <v>31</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L48" s="2">
         <v>0</v>
@@ -13217,16 +13217,16 @@
         <v>45139</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F49" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="G49">
         <v>120</v>
@@ -13465,7 +13465,7 @@
         <v>45139</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D50" t="s">
         <v>32</v>
@@ -13474,7 +13474,7 @@
         <v>29</v>
       </c>
       <c r="F50" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="G50">
         <v>120</v>
@@ -13489,7 +13489,7 @@
         <v>31</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L50" s="2">
         <v>0</v>
@@ -13713,7 +13713,7 @@
         <v>45139</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D51" t="s">
         <v>32</v>
@@ -13722,7 +13722,7 @@
         <v>28</v>
       </c>
       <c r="F51" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="G51">
         <v>120</v>
@@ -13737,7 +13737,7 @@
         <v>31</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L51" s="2">
         <v>0</v>
@@ -13961,16 +13961,16 @@
         <v>45139</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D52" t="s">
         <v>32</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>249</v>
+        <v>225</v>
       </c>
       <c r="F52" t="s">
-        <v>101</v>
+        <v>245</v>
       </c>
       <c r="G52">
         <v>120</v>
@@ -13985,7 +13985,7 @@
         <v>31</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L52" s="2">
         <v>0</v>
@@ -14209,7 +14209,7 @@
         <v>45139</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D53" t="s">
         <v>32</v>
@@ -14218,7 +14218,7 @@
         <v>31</v>
       </c>
       <c r="F53" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="G53">
         <v>120</v>
@@ -14233,7 +14233,7 @@
         <v>31</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L53" s="2">
         <v>0</v>
@@ -14457,16 +14457,16 @@
         <v>45139</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D54" t="s">
         <v>32</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>250</v>
+        <v>226</v>
       </c>
       <c r="F54" t="s">
-        <v>103</v>
+        <v>246</v>
       </c>
       <c r="G54">
         <v>120</v>
@@ -14481,7 +14481,7 @@
         <v>31</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L54" s="2">
         <v>0</v>
@@ -14705,16 +14705,16 @@
         <v>45139</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D55" t="s">
         <v>32</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F55" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="G55">
         <v>120</v>
@@ -14729,7 +14729,7 @@
         <v>31</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L55" s="2">
         <v>0</v>
@@ -14953,7 +14953,7 @@
         <v>45139</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D56" t="s">
         <v>32</v>
@@ -14962,7 +14962,7 @@
         <v>34</v>
       </c>
       <c r="F56" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="G56">
         <v>120</v>
@@ -14977,7 +14977,7 @@
         <v>31</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L56" s="2">
         <v>0</v>
@@ -15201,16 +15201,16 @@
         <v>45139</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F57" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="G57">
         <v>120</v>
@@ -15449,16 +15449,16 @@
         <v>45139</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D58" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E58" s="6" t="s">
         <v>29</v>
       </c>
       <c r="F58" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="G58">
         <v>120</v>
@@ -15473,7 +15473,7 @@
         <v>31</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L58" s="2">
         <v>0</v>
@@ -15697,16 +15697,16 @@
         <v>45139</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D59" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E59" s="6" t="s">
         <v>28</v>
       </c>
       <c r="F59" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="G59">
         <v>120</v>
@@ -15721,7 +15721,7 @@
         <v>31</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L59" s="2">
         <v>0</v>
@@ -15945,16 +15945,16 @@
         <v>45139</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D60" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E60" s="6" t="s">
         <v>31</v>
       </c>
       <c r="F60" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="G60">
         <v>120</v>
@@ -15969,7 +15969,7 @@
         <v>31</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L60" s="2">
         <v>0</v>
@@ -16193,16 +16193,16 @@
         <v>45139</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F61" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="G61">
         <v>120</v>
@@ -16441,7 +16441,7 @@
         <v>45139</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D62" t="s">
         <v>31</v>
@@ -16450,7 +16450,7 @@
         <v>29</v>
       </c>
       <c r="F62" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="G62">
         <v>120</v>
@@ -16465,7 +16465,7 @@
         <v>31</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L62" s="2">
         <v>0</v>
@@ -16689,16 +16689,16 @@
         <v>45139</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D63" t="s">
         <v>31</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F63" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="G63">
         <v>120</v>
@@ -16713,7 +16713,7 @@
         <v>31</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L63" s="2">
         <v>0</v>
@@ -16937,16 +16937,16 @@
         <v>45139</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D64" t="s">
         <v>31</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="F64" t="s">
-        <v>110</v>
+        <v>247</v>
       </c>
       <c r="G64">
         <v>120</v>
@@ -16961,7 +16961,7 @@
         <v>31</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L64" s="2">
         <v>0</v>
@@ -17185,16 +17185,16 @@
         <v>45139</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D65" t="s">
         <v>31</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F65" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="G65">
         <v>120</v>
@@ -17209,7 +17209,7 @@
         <v>31</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L65" s="2">
         <v>0</v>
@@ -17433,16 +17433,16 @@
         <v>45139</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D66" t="s">
         <v>31</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>252</v>
+        <v>228</v>
       </c>
       <c r="F66" t="s">
-        <v>112</v>
+        <v>248</v>
       </c>
       <c r="G66">
         <v>120</v>
@@ -17457,7 +17457,7 @@
         <v>31</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L66" s="2">
         <v>0</v>
@@ -17681,16 +17681,16 @@
         <v>45139</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D67" t="s">
         <v>31</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F67" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="G67">
         <v>120</v>
@@ -17705,7 +17705,7 @@
         <v>31</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L67" s="2">
         <v>0</v>
@@ -17929,16 +17929,16 @@
         <v>45139</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D68" t="s">
         <v>31</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F68" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="G68">
         <v>120</v>
@@ -17953,7 +17953,7 @@
         <v>31</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L68" s="2">
         <v>0</v>
@@ -18177,16 +18177,16 @@
         <v>45139</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F69" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="G69">
         <v>120</v>
@@ -18201,7 +18201,7 @@
         <v>31</v>
       </c>
       <c r="K69" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L69" s="2">
         <v>0</v>
@@ -18425,7 +18425,7 @@
         <v>45139</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D70" t="s">
         <v>33</v>
@@ -18434,7 +18434,7 @@
         <v>29</v>
       </c>
       <c r="F70" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="G70">
         <v>120</v>
@@ -18449,7 +18449,7 @@
         <v>31</v>
       </c>
       <c r="K70" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L70" s="2">
         <v>0</v>
@@ -18673,16 +18673,16 @@
         <v>45139</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D71" t="s">
         <v>33</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F71" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="G71">
         <v>120</v>
@@ -18697,7 +18697,7 @@
         <v>31</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L71" s="2">
         <v>0</v>
@@ -18921,16 +18921,16 @@
         <v>45139</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D72" t="s">
         <v>33</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="F72" t="s">
-        <v>118</v>
+        <v>249</v>
       </c>
       <c r="G72">
         <v>120</v>
@@ -18945,7 +18945,7 @@
         <v>31</v>
       </c>
       <c r="K72" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L72" s="2">
         <v>0</v>
@@ -19169,16 +19169,16 @@
         <v>45139</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D73" t="s">
         <v>33</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F73" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="G73">
         <v>120</v>
@@ -19193,7 +19193,7 @@
         <v>31</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L73" s="2">
         <v>0</v>
@@ -19417,16 +19417,16 @@
         <v>45139</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D74" t="s">
         <v>33</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>252</v>
+        <v>228</v>
       </c>
       <c r="F74" t="s">
-        <v>120</v>
+        <v>250</v>
       </c>
       <c r="G74">
         <v>120</v>
@@ -19441,7 +19441,7 @@
         <v>31</v>
       </c>
       <c r="K74" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L74" s="2">
         <v>0</v>
@@ -19665,16 +19665,16 @@
         <v>45139</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D75" t="s">
         <v>33</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F75" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="G75">
         <v>120</v>
@@ -19689,7 +19689,7 @@
         <v>31</v>
       </c>
       <c r="K75" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L75" s="2">
         <v>0</v>
@@ -19913,16 +19913,16 @@
         <v>45139</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D76" t="s">
         <v>33</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F76" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="G76">
         <v>120</v>
@@ -19937,7 +19937,7 @@
         <v>31</v>
       </c>
       <c r="K76" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L76" s="2">
         <v>0</v>
@@ -20161,16 +20161,16 @@
         <v>45139</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F77" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="G77">
         <v>120</v>
@@ -20185,7 +20185,7 @@
         <v>31</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L77" s="2">
         <v>0</v>
@@ -20409,16 +20409,16 @@
         <v>45139</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D78" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E78" s="6" t="s">
         <v>29</v>
       </c>
       <c r="F78" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="G78">
         <v>120</v>
@@ -20433,7 +20433,7 @@
         <v>31</v>
       </c>
       <c r="K78" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L78" s="2">
         <v>0</v>
@@ -20657,16 +20657,16 @@
         <v>45139</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E79" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F79" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="G79">
         <v>120</v>
@@ -20681,7 +20681,7 @@
         <v>31</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L79" s="2">
         <v>0</v>
@@ -20905,16 +20905,16 @@
         <v>45139</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F80" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="G80">
         <v>120</v>
@@ -20929,7 +20929,7 @@
         <v>31</v>
       </c>
       <c r="K80" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L80" s="2">
         <v>0</v>
@@ -21153,16 +21153,16 @@
         <v>45139</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F81" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="G81">
         <v>120</v>
@@ -21401,7 +21401,7 @@
         <v>45139</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>28</v>
@@ -21410,7 +21410,7 @@
         <v>29</v>
       </c>
       <c r="F82" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="G82">
         <v>120</v>
@@ -21649,7 +21649,7 @@
         <v>45139</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>28</v>
@@ -21658,7 +21658,7 @@
         <v>28</v>
       </c>
       <c r="F83" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="G83">
         <v>120</v>
@@ -21897,16 +21897,16 @@
         <v>45139</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>249</v>
+        <v>225</v>
       </c>
       <c r="F84" t="s">
-        <v>129</v>
+        <v>251</v>
       </c>
       <c r="G84">
         <v>120</v>
@@ -22145,7 +22145,7 @@
         <v>45139</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>28</v>
@@ -22154,7 +22154,7 @@
         <v>31</v>
       </c>
       <c r="F85" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="G85">
         <v>120</v>
@@ -22393,16 +22393,16 @@
         <v>45139</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E86" s="6" t="s">
-        <v>250</v>
+        <v>226</v>
       </c>
       <c r="F86" t="s">
-        <v>131</v>
+        <v>252</v>
       </c>
       <c r="G86">
         <v>120</v>
@@ -22641,16 +22641,16 @@
         <v>45139</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F87" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="G87">
         <v>120</v>
@@ -22889,7 +22889,7 @@
         <v>45139</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>28</v>
@@ -22898,7 +22898,7 @@
         <v>34</v>
       </c>
       <c r="F88" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
       <c r="G88">
         <v>120</v>
@@ -23137,16 +23137,16 @@
         <v>45139</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F89" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="G89">
         <v>120</v>
@@ -23263,7 +23263,7 @@
         <v>1</v>
       </c>
       <c r="AS89" s="7" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="AT89">
         <v>0</v>
@@ -23317,13 +23317,13 @@
         <v>0</v>
       </c>
       <c r="BK89" s="2" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="BL89">
         <v>1</v>
       </c>
       <c r="BM89" s="7" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="BN89">
         <v>0</v>
@@ -23385,7 +23385,7 @@
         <v>45139</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>32</v>
@@ -23394,7 +23394,7 @@
         <v>29</v>
       </c>
       <c r="F90" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="G90">
         <v>120</v>
@@ -23633,7 +23633,7 @@
         <v>45139</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>32</v>
@@ -23642,7 +23642,7 @@
         <v>28</v>
       </c>
       <c r="F91" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="G91">
         <v>120</v>
@@ -23881,16 +23881,16 @@
         <v>45139</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>249</v>
+        <v>225</v>
       </c>
       <c r="F92" t="s">
-        <v>140</v>
+        <v>253</v>
       </c>
       <c r="G92">
         <v>120</v>
@@ -24129,7 +24129,7 @@
         <v>45139</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>32</v>
@@ -24138,7 +24138,7 @@
         <v>31</v>
       </c>
       <c r="F93" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="G93">
         <v>120</v>
@@ -24377,16 +24377,16 @@
         <v>45139</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E94" s="6" t="s">
-        <v>250</v>
+        <v>226</v>
       </c>
       <c r="F94" t="s">
-        <v>142</v>
+        <v>254</v>
       </c>
       <c r="G94">
         <v>120</v>
@@ -24625,16 +24625,16 @@
         <v>45139</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E95" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F95" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="G95">
         <v>120</v>
@@ -24873,7 +24873,7 @@
         <v>45139</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>32</v>
@@ -24882,7 +24882,7 @@
         <v>34</v>
       </c>
       <c r="F96" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
       <c r="G96">
         <v>120</v>
@@ -25121,16 +25121,16 @@
         <v>45139</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F97" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="G97">
         <v>120</v>
@@ -25247,7 +25247,7 @@
         <v>1</v>
       </c>
       <c r="AS97" s="7" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="AT97">
         <v>0</v>
@@ -25301,13 +25301,13 @@
         <v>0</v>
       </c>
       <c r="BK97" s="2" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="BL97">
         <v>1</v>
       </c>
       <c r="BM97" s="7" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="BN97">
         <v>0</v>
@@ -25369,16 +25369,16 @@
         <v>45139</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D98" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E98" s="9" t="s">
         <v>29</v>
       </c>
       <c r="F98" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="G98">
         <v>120</v>
@@ -25617,16 +25617,16 @@
         <v>45139</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D99" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E99" s="6" t="s">
         <v>28</v>
       </c>
       <c r="F99" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
       <c r="G99">
         <v>120</v>
@@ -25865,16 +25865,16 @@
         <v>45139</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D100" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E100" s="6" t="s">
         <v>31</v>
       </c>
       <c r="F100" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
       <c r="G100">
         <v>120</v>
@@ -26113,16 +26113,16 @@
         <v>45139</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D101" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F101" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="G101">
         <v>120</v>
@@ -26239,7 +26239,7 @@
         <v>1</v>
       </c>
       <c r="AS101" s="7" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="AT101">
         <v>0</v>
@@ -26293,13 +26293,13 @@
         <v>0</v>
       </c>
       <c r="BK101" s="2" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="BL101">
         <v>1</v>
       </c>
       <c r="BM101" s="7" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="BN101">
         <v>0</v>
@@ -26361,7 +26361,7 @@
         <v>45139</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D102" t="s">
         <v>31</v>
@@ -26370,7 +26370,7 @@
         <v>29</v>
       </c>
       <c r="F102" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
       <c r="G102">
         <v>120</v>
@@ -26609,16 +26609,16 @@
         <v>45139</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D103" t="s">
         <v>31</v>
       </c>
       <c r="E103" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F103" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="G103">
         <v>120</v>
@@ -26857,16 +26857,16 @@
         <v>45139</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D104" t="s">
         <v>31</v>
       </c>
       <c r="E104" s="6" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="F104" t="s">
-        <v>150</v>
+        <v>255</v>
       </c>
       <c r="G104">
         <v>120</v>
@@ -27105,16 +27105,16 @@
         <v>45139</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D105" t="s">
         <v>31</v>
       </c>
       <c r="E105" s="6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F105" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="G105">
         <v>120</v>
@@ -27353,16 +27353,16 @@
         <v>45139</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D106" t="s">
         <v>31</v>
       </c>
       <c r="E106" s="6" t="s">
-        <v>252</v>
+        <v>228</v>
       </c>
       <c r="F106" t="s">
-        <v>152</v>
+        <v>256</v>
       </c>
       <c r="G106">
         <v>120</v>
@@ -27601,16 +27601,16 @@
         <v>45139</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D107" t="s">
         <v>31</v>
       </c>
       <c r="E107" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F107" t="s">
-        <v>153</v>
+        <v>131</v>
       </c>
       <c r="G107">
         <v>120</v>
@@ -27849,16 +27849,16 @@
         <v>45139</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D108" t="s">
         <v>31</v>
       </c>
       <c r="E108" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F108" t="s">
-        <v>154</v>
+        <v>132</v>
       </c>
       <c r="G108">
         <v>120</v>
@@ -28097,16 +28097,16 @@
         <v>45139</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D109" t="s">
         <v>31</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F109" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="G109">
         <v>120</v>
@@ -28223,7 +28223,7 @@
         <v>1</v>
       </c>
       <c r="AS109" s="7" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="AT109">
         <v>0</v>
@@ -28277,13 +28277,13 @@
         <v>0</v>
       </c>
       <c r="BK109" s="2" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="BL109">
         <v>1</v>
       </c>
       <c r="BM109" s="7" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="BN109">
         <v>0</v>
@@ -28345,7 +28345,7 @@
         <v>45139</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D110" t="s">
         <v>33</v>
@@ -28354,7 +28354,7 @@
         <v>29</v>
       </c>
       <c r="F110" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="G110">
         <v>120</v>
@@ -28593,16 +28593,16 @@
         <v>45139</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D111" t="s">
         <v>33</v>
       </c>
       <c r="E111" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F111" t="s">
-        <v>156</v>
+        <v>134</v>
       </c>
       <c r="G111">
         <v>120</v>
@@ -28841,16 +28841,16 @@
         <v>45139</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D112" t="s">
         <v>33</v>
       </c>
       <c r="E112" s="6" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="F112" t="s">
-        <v>157</v>
+        <v>257</v>
       </c>
       <c r="G112">
         <v>120</v>
@@ -29089,16 +29089,16 @@
         <v>45139</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D113" t="s">
         <v>33</v>
       </c>
       <c r="E113" s="6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F113" t="s">
-        <v>158</v>
+        <v>135</v>
       </c>
       <c r="G113">
         <v>120</v>
@@ -29337,16 +29337,16 @@
         <v>45139</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D114" t="s">
         <v>33</v>
       </c>
       <c r="E114" s="6" t="s">
-        <v>252</v>
+        <v>228</v>
       </c>
       <c r="F114" t="s">
-        <v>159</v>
+        <v>258</v>
       </c>
       <c r="G114">
         <v>120</v>
@@ -29585,16 +29585,16 @@
         <v>45139</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D115" t="s">
         <v>33</v>
       </c>
       <c r="E115" s="9" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F115" t="s">
-        <v>160</v>
+        <v>136</v>
       </c>
       <c r="G115">
         <v>120</v>
@@ -29833,16 +29833,16 @@
         <v>45139</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D116" t="s">
         <v>33</v>
       </c>
       <c r="E116" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F116" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="G116">
         <v>120</v>
@@ -30081,16 +30081,16 @@
         <v>45139</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D117" t="s">
         <v>33</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F117" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="G117">
         <v>120</v>
@@ -30207,7 +30207,7 @@
         <v>1</v>
       </c>
       <c r="AS117" s="7" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="AT117">
         <v>0</v>
@@ -30261,13 +30261,13 @@
         <v>0</v>
       </c>
       <c r="BK117" s="2" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="BL117">
         <v>1</v>
       </c>
       <c r="BM117" s="7" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="BN117">
         <v>0</v>
@@ -30329,16 +30329,16 @@
         <v>45139</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D118" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E118" s="9" t="s">
         <v>29</v>
       </c>
       <c r="F118" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="G118">
         <v>120</v>
@@ -30577,16 +30577,16 @@
         <v>45139</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F119" t="s">
-        <v>163</v>
+        <v>139</v>
       </c>
       <c r="G119">
         <v>120</v>
@@ -30825,16 +30825,16 @@
         <v>45139</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F120" t="s">
-        <v>164</v>
+        <v>140</v>
       </c>
       <c r="G120">
         <v>120</v>
@@ -31073,16 +31073,16 @@
         <v>45139</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F121" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="G121">
         <v>120</v>
@@ -31199,7 +31199,7 @@
         <v>1</v>
       </c>
       <c r="AS121" s="7" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="AT121">
         <v>0</v>
@@ -31253,13 +31253,13 @@
         <v>0</v>
       </c>
       <c r="BK121" s="2" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="BL121">
         <v>1</v>
       </c>
       <c r="BM121" s="7" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="BN121">
         <v>0</v>
@@ -31318,16 +31318,16 @@
         <v>45139</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>165</v>
+        <v>141</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
       <c r="E122" s="3" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="F122" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="G122">
         <v>240</v>
@@ -31360,10 +31360,10 @@
         <v>36</v>
       </c>
       <c r="Q122" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="R122" s="2" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="S122" s="2">
         <v>0</v>
@@ -31566,16 +31566,16 @@
         <v>45139</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>165</v>
+        <v>141</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
       <c r="E123" s="3" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="F123" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="G123">
         <v>240</v>
@@ -31608,10 +31608,10 @@
         <v>36</v>
       </c>
       <c r="Q123" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="R123" s="2" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="S123" s="2">
         <v>0</v>
@@ -31814,16 +31814,16 @@
         <v>45139</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>165</v>
+        <v>141</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>253</v>
+        <v>229</v>
       </c>
       <c r="E124" s="3" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="F124" s="8" t="s">
-        <v>255</v>
+        <v>231</v>
       </c>
       <c r="G124">
         <v>240</v>
@@ -31856,10 +31856,10 @@
         <v>36</v>
       </c>
       <c r="Q124" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="R124" s="2" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="S124" s="2">
         <v>0</v>
@@ -32062,16 +32062,16 @@
         <v>45139</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>165</v>
+        <v>141</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>173</v>
+        <v>149</v>
       </c>
       <c r="E125" s="3" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="F125" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="G125">
         <v>240</v>
@@ -32104,10 +32104,10 @@
         <v>36</v>
       </c>
       <c r="Q125" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="R125" s="2" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="S125" s="2">
         <v>0</v>
@@ -32310,16 +32310,16 @@
         <v>45139</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>165</v>
+        <v>141</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>173</v>
+        <v>149</v>
       </c>
       <c r="E126" s="3" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="F126" t="s">
-        <v>175</v>
+        <v>151</v>
       </c>
       <c r="G126">
         <v>240</v>
@@ -32352,10 +32352,10 @@
         <v>36</v>
       </c>
       <c r="Q126" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="R126" s="2" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="S126" s="2">
         <v>0</v>
@@ -32558,16 +32558,16 @@
         <v>45139</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>165</v>
+        <v>141</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
       <c r="E127" s="3" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="F127" s="8" t="s">
-        <v>256</v>
+        <v>232</v>
       </c>
       <c r="G127">
         <v>240</v>
@@ -32600,10 +32600,10 @@
         <v>36</v>
       </c>
       <c r="Q127" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="R127" s="2" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="S127" s="2">
         <v>0</v>
@@ -32806,16 +32806,16 @@
         <v>45139</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>165</v>
+        <v>141</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>176</v>
+        <v>152</v>
       </c>
       <c r="E128" s="3" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="F128" t="s">
-        <v>177</v>
+        <v>153</v>
       </c>
       <c r="G128">
         <v>240</v>
@@ -32848,10 +32848,10 @@
         <v>36</v>
       </c>
       <c r="Q128" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="R128" s="2" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="S128" s="2">
         <v>0</v>
@@ -33054,16 +33054,16 @@
         <v>45139</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>165</v>
+        <v>141</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>176</v>
+        <v>152</v>
       </c>
       <c r="E129" s="3" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="F129" t="s">
-        <v>178</v>
+        <v>154</v>
       </c>
       <c r="G129">
         <v>240</v>
@@ -33096,10 +33096,10 @@
         <v>36</v>
       </c>
       <c r="Q129" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="R129" s="2" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="S129" s="2">
         <v>0</v>
@@ -33302,16 +33302,16 @@
         <v>45139</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>165</v>
+        <v>141</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="F130" t="s">
-        <v>180</v>
+        <v>156</v>
       </c>
       <c r="G130">
         <v>240</v>
@@ -33344,10 +33344,10 @@
         <v>36</v>
       </c>
       <c r="Q130" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="R130" s="2" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="S130" s="2">
         <v>0</v>
@@ -33550,16 +33550,16 @@
         <v>45139</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>165</v>
+        <v>141</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="E131" s="3" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="F131" t="s">
-        <v>181</v>
+        <v>157</v>
       </c>
       <c r="G131">
         <v>240</v>
@@ -33592,10 +33592,10 @@
         <v>36</v>
       </c>
       <c r="Q131" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="R131" s="2" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="S131" s="2">
         <v>0</v>
@@ -33798,16 +33798,16 @@
         <v>45139</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="F132" t="s">
-        <v>183</v>
+        <v>159</v>
       </c>
       <c r="G132">
         <v>240</v>
@@ -33840,10 +33840,10 @@
         <v>36</v>
       </c>
       <c r="Q132" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="R132" s="2" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="S132" s="2">
         <v>0</v>
@@ -34046,16 +34046,16 @@
         <v>45139</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
       <c r="E133" s="3" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="F133" t="s">
-        <v>184</v>
+        <v>160</v>
       </c>
       <c r="G133">
         <v>240</v>
@@ -34088,10 +34088,10 @@
         <v>36</v>
       </c>
       <c r="Q133" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="R133" s="2" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="S133" s="2">
         <v>0</v>
@@ -34294,16 +34294,16 @@
         <v>45139</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>253</v>
+        <v>229</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="F134" s="8" t="s">
-        <v>257</v>
+        <v>233</v>
       </c>
       <c r="G134">
         <v>240</v>
@@ -34336,10 +34336,10 @@
         <v>36</v>
       </c>
       <c r="Q134" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="R134" s="2" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="S134" s="2">
         <v>0</v>
@@ -34542,16 +34542,16 @@
         <v>45139</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>173</v>
+        <v>149</v>
       </c>
       <c r="E135" s="3" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="F135" t="s">
-        <v>185</v>
+        <v>161</v>
       </c>
       <c r="G135">
         <v>240</v>
@@ -34584,10 +34584,10 @@
         <v>36</v>
       </c>
       <c r="Q135" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="R135" s="2" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="S135" s="2">
         <v>0</v>
@@ -34790,16 +34790,16 @@
         <v>45139</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>173</v>
+        <v>149</v>
       </c>
       <c r="E136" s="3" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="F136" t="s">
-        <v>186</v>
+        <v>162</v>
       </c>
       <c r="G136">
         <v>240</v>
@@ -34832,10 +34832,10 @@
         <v>36</v>
       </c>
       <c r="Q136" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="R136" s="2" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="S136" s="2">
         <v>0</v>
@@ -35038,16 +35038,16 @@
         <v>45139</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
       <c r="E137" s="3" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="F137" s="8" t="s">
-        <v>258</v>
+        <v>234</v>
       </c>
       <c r="G137">
         <v>240</v>
@@ -35080,10 +35080,10 @@
         <v>36</v>
       </c>
       <c r="Q137" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="R137" s="2" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="S137" s="2">
         <v>0</v>
@@ -35286,16 +35286,16 @@
         <v>45139</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>176</v>
+        <v>152</v>
       </c>
       <c r="E138" s="3" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="F138" t="s">
-        <v>187</v>
+        <v>163</v>
       </c>
       <c r="G138">
         <v>240</v>
@@ -35328,10 +35328,10 @@
         <v>36</v>
       </c>
       <c r="Q138" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="R138" s="2" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="S138" s="2">
         <v>0</v>
@@ -35534,16 +35534,16 @@
         <v>45139</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>176</v>
+        <v>152</v>
       </c>
       <c r="E139" s="3" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="F139" t="s">
-        <v>188</v>
+        <v>164</v>
       </c>
       <c r="G139">
         <v>240</v>
@@ -35576,10 +35576,10 @@
         <v>36</v>
       </c>
       <c r="Q139" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="R139" s="2" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="S139" s="2">
         <v>0</v>
@@ -35782,16 +35782,16 @@
         <v>45139</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="F140" t="s">
-        <v>189</v>
+        <v>165</v>
       </c>
       <c r="G140">
         <v>240</v>
@@ -35824,10 +35824,10 @@
         <v>36</v>
       </c>
       <c r="Q140" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="R140" s="2" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="S140" s="2">
         <v>0</v>
@@ -36030,16 +36030,16 @@
         <v>45139</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="E141" s="3" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="F141" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
       <c r="G141">
         <v>240</v>
@@ -36072,10 +36072,10 @@
         <v>36</v>
       </c>
       <c r="Q141" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="R141" s="2" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="S141" s="2">
         <v>0</v>
@@ -36278,16 +36278,16 @@
         <v>45139</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>192</v>
+        <v>168</v>
       </c>
       <c r="E142" s="3" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="F142" t="s">
-        <v>193</v>
+        <v>169</v>
       </c>
       <c r="G142">
         <v>240</v>
@@ -36305,7 +36305,7 @@
         <v>32</v>
       </c>
       <c r="L142" s="2" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="M142" s="2" t="s">
         <v>31</v>
@@ -36320,10 +36320,10 @@
         <v>36</v>
       </c>
       <c r="Q142" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="R142" s="2" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="S142" s="2">
         <v>0</v>
@@ -36526,16 +36526,16 @@
         <v>45139</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>192</v>
+        <v>168</v>
       </c>
       <c r="E143" s="3" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="F143" t="s">
-        <v>194</v>
+        <v>170</v>
       </c>
       <c r="G143">
         <v>240</v>
@@ -36553,7 +36553,7 @@
         <v>32</v>
       </c>
       <c r="L143" s="2" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="M143" s="2" t="s">
         <v>31</v>
@@ -36568,10 +36568,10 @@
         <v>36</v>
       </c>
       <c r="Q143" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="R143" s="2" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="S143" s="2">
         <v>0</v>
@@ -36774,16 +36774,16 @@
         <v>45139</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E144" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="F144" t="s">
         <v>171</v>
-      </c>
-      <c r="F144" t="s">
-        <v>195</v>
       </c>
       <c r="G144">
         <v>240</v>
@@ -36801,7 +36801,7 @@
         <v>32</v>
       </c>
       <c r="L144" s="2" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="M144" s="2" t="s">
         <v>31</v>
@@ -36816,10 +36816,10 @@
         <v>36</v>
       </c>
       <c r="Q144" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="R144" s="2" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="S144" s="2">
         <v>0</v>
@@ -37022,16 +37022,16 @@
         <v>45139</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E145" s="3" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="F145" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
       <c r="G145">
         <v>240</v>
@@ -37049,7 +37049,7 @@
         <v>32</v>
       </c>
       <c r="L145" s="2" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="M145" s="2" t="s">
         <v>31</v>
@@ -37064,10 +37064,10 @@
         <v>36</v>
       </c>
       <c r="Q145" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="R145" s="2" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="S145" s="2">
         <v>0</v>
@@ -37270,16 +37270,16 @@
         <v>45139</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="E146" s="3" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="F146" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
       <c r="G146">
         <v>240</v>
@@ -37297,7 +37297,7 @@
         <v>32</v>
       </c>
       <c r="L146" s="2" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="M146" s="2" t="s">
         <v>31</v>
@@ -37312,10 +37312,10 @@
         <v>36</v>
       </c>
       <c r="Q146" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="R146" s="2" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="S146" s="2">
         <v>0</v>
@@ -37518,16 +37518,16 @@
         <v>45139</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="E147" s="3" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="F147" t="s">
-        <v>200</v>
+        <v>176</v>
       </c>
       <c r="G147">
         <v>240</v>
@@ -37545,7 +37545,7 @@
         <v>32</v>
       </c>
       <c r="L147" s="2" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="M147" s="2" t="s">
         <v>31</v>
@@ -37560,10 +37560,10 @@
         <v>36</v>
       </c>
       <c r="Q147" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="R147" s="2" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="S147" s="2">
         <v>0</v>
@@ -37766,16 +37766,16 @@
         <v>45139</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>201</v>
+        <v>177</v>
       </c>
       <c r="E148" s="3" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="F148" t="s">
-        <v>202</v>
+        <v>178</v>
       </c>
       <c r="G148">
         <v>240</v>
@@ -37793,7 +37793,7 @@
         <v>32</v>
       </c>
       <c r="L148" s="2" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="M148" s="2" t="s">
         <v>31</v>
@@ -37808,10 +37808,10 @@
         <v>36</v>
       </c>
       <c r="Q148" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="R148" s="2" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="S148" s="2">
         <v>0</v>
@@ -38014,16 +38014,16 @@
         <v>45139</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>201</v>
+        <v>177</v>
       </c>
       <c r="E149" s="3" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="F149" t="s">
-        <v>203</v>
+        <v>179</v>
       </c>
       <c r="G149">
         <v>240</v>
@@ -38041,7 +38041,7 @@
         <v>32</v>
       </c>
       <c r="L149" s="2" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="M149" s="2" t="s">
         <v>31</v>
@@ -38056,10 +38056,10 @@
         <v>36</v>
       </c>
       <c r="Q149" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="R149" s="2" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="S149" s="2">
         <v>0</v>
@@ -38262,16 +38262,16 @@
         <v>45139</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>204</v>
+        <v>180</v>
       </c>
       <c r="E150" s="3" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="F150" t="s">
-        <v>205</v>
+        <v>181</v>
       </c>
       <c r="G150">
         <v>240</v>
@@ -38289,7 +38289,7 @@
         <v>32</v>
       </c>
       <c r="L150" s="2" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="M150" s="2" t="s">
         <v>31</v>
@@ -38304,10 +38304,10 @@
         <v>36</v>
       </c>
       <c r="Q150" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="R150" s="2" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="S150" s="2">
         <v>0</v>
@@ -38510,16 +38510,16 @@
         <v>45139</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>204</v>
+        <v>180</v>
       </c>
       <c r="E151" s="3" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="F151" t="s">
-        <v>206</v>
+        <v>182</v>
       </c>
       <c r="G151">
         <v>240</v>
@@ -38537,7 +38537,7 @@
         <v>32</v>
       </c>
       <c r="L151" s="2" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="M151" s="2" t="s">
         <v>31</v>
@@ -38552,10 +38552,10 @@
         <v>36</v>
       </c>
       <c r="Q151" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="R151" s="2" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="S151" s="2">
         <v>0</v>
@@ -38758,16 +38758,16 @@
         <v>45139</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>207</v>
+        <v>183</v>
       </c>
       <c r="E152" s="3" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="F152" t="s">
-        <v>208</v>
+        <v>184</v>
       </c>
       <c r="G152">
         <v>240</v>
@@ -38785,7 +38785,7 @@
         <v>32</v>
       </c>
       <c r="L152" s="2" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="M152" s="2" t="s">
         <v>31</v>
@@ -38800,10 +38800,10 @@
         <v>36</v>
       </c>
       <c r="Q152" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="R152" s="2" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="S152" s="2">
         <v>0</v>
@@ -39006,16 +39006,16 @@
         <v>45139</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>207</v>
+        <v>183</v>
       </c>
       <c r="E153" s="3" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="F153" t="s">
-        <v>209</v>
+        <v>185</v>
       </c>
       <c r="G153">
         <v>240</v>
@@ -39033,7 +39033,7 @@
         <v>32</v>
       </c>
       <c r="L153" s="2" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="M153" s="2" t="s">
         <v>31</v>
@@ -39048,10 +39048,10 @@
         <v>36</v>
       </c>
       <c r="Q153" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="R153" s="2" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="S153" s="2">
         <v>0</v>
@@ -39254,16 +39254,16 @@
         <v>45139</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>210</v>
+        <v>186</v>
       </c>
       <c r="D154" t="s">
-        <v>192</v>
+        <v>168</v>
       </c>
       <c r="E154" s="10" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="F154" t="s">
-        <v>211</v>
+        <v>187</v>
       </c>
       <c r="G154">
         <v>240</v>
@@ -39281,7 +39281,7 @@
         <v>32</v>
       </c>
       <c r="L154" s="2" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="M154" s="2" t="s">
         <v>31</v>
@@ -39296,10 +39296,10 @@
         <v>36</v>
       </c>
       <c r="Q154" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="R154" s="2" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="S154" s="2">
         <v>0</v>
@@ -39502,16 +39502,16 @@
         <v>45139</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>210</v>
+        <v>186</v>
       </c>
       <c r="D155" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E155" s="10" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="F155" t="s">
-        <v>211</v>
+        <v>187</v>
       </c>
       <c r="G155">
         <v>240</v>
@@ -39529,7 +39529,7 @@
         <v>32</v>
       </c>
       <c r="L155" s="2" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="M155" s="2" t="s">
         <v>31</v>
@@ -39544,10 +39544,10 @@
         <v>36</v>
       </c>
       <c r="Q155" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="R155" s="2" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="S155" s="2">
         <v>0</v>
@@ -39750,10 +39750,10 @@
         <v>45139</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>212</v>
+        <v>188</v>
       </c>
       <c r="F156" t="s">
-        <v>213</v>
+        <v>189</v>
       </c>
       <c r="G156">
         <v>210</v>
@@ -39837,7 +39837,7 @@
         <v>0</v>
       </c>
       <c r="AH156" s="2" t="s">
-        <v>214</v>
+        <v>190</v>
       </c>
       <c r="AI156">
         <v>0</v>
@@ -39992,10 +39992,10 @@
         <v>45139</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>215</v>
+        <v>191</v>
       </c>
       <c r="F157" t="s">
-        <v>216</v>
+        <v>192</v>
       </c>
       <c r="G157">
         <v>190</v>
@@ -40234,10 +40234,10 @@
         <v>45139</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="F158" t="s">
-        <v>218</v>
+        <v>194</v>
       </c>
       <c r="G158">
         <v>220</v>
@@ -40255,7 +40255,7 @@
         <v>32</v>
       </c>
       <c r="L158" s="2" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="M158" s="2">
         <v>0</v>
@@ -40270,10 +40270,10 @@
         <v>36</v>
       </c>
       <c r="Q158" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="R158" s="2" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="S158" s="2">
         <v>0</v>
@@ -40476,10 +40476,10 @@
         <v>45139</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="F159" s="8" t="s">
-        <v>247</v>
+        <v>223</v>
       </c>
       <c r="G159">
         <v>170</v>
@@ -40497,7 +40497,7 @@
         <v>32</v>
       </c>
       <c r="L159" s="2" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="M159" s="2">
         <v>0</v>
@@ -40512,13 +40512,13 @@
         <v>36</v>
       </c>
       <c r="Q159" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="R159" s="2" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="S159" s="2" t="s">
-        <v>220</v>
+        <v>196</v>
       </c>
       <c r="T159" s="2">
         <v>0</v>
@@ -40718,10 +40718,10 @@
         <v>45139</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>221</v>
+        <v>197</v>
       </c>
       <c r="F160" t="s">
-        <v>222</v>
+        <v>198</v>
       </c>
       <c r="G160">
         <v>190</v>
@@ -40739,7 +40739,7 @@
         <v>32</v>
       </c>
       <c r="L160" s="2" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="M160" s="2">
         <v>0</v>
@@ -40754,10 +40754,10 @@
         <v>36</v>
       </c>
       <c r="Q160" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="R160" s="2" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="S160" s="2">
         <v>0</v>
@@ -40960,10 +40960,10 @@
         <v>45139</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>223</v>
+        <v>199</v>
       </c>
       <c r="F161" t="s">
-        <v>224</v>
+        <v>200</v>
       </c>
       <c r="G161">
         <v>220</v>
@@ -41202,13 +41202,13 @@
         <v>45139</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>225</v>
+        <v>201</v>
       </c>
       <c r="D162" t="s">
-        <v>226</v>
+        <v>202</v>
       </c>
       <c r="F162" t="s">
-        <v>227</v>
+        <v>203</v>
       </c>
       <c r="G162">
         <v>220</v>
@@ -41447,13 +41447,13 @@
         <v>45139</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>225</v>
+        <v>201</v>
       </c>
       <c r="D163" t="s">
-        <v>228</v>
+        <v>204</v>
       </c>
       <c r="F163" t="s">
-        <v>229</v>
+        <v>205</v>
       </c>
       <c r="G163">
         <v>220</v>
@@ -41692,10 +41692,10 @@
         <v>45139</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>230</v>
+        <v>206</v>
       </c>
       <c r="F164" t="s">
-        <v>231</v>
+        <v>207</v>
       </c>
       <c r="G164">
         <v>240</v>
@@ -41719,7 +41719,7 @@
         <v>0</v>
       </c>
       <c r="N164" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="O164" s="2">
         <v>0</v>
@@ -41934,10 +41934,10 @@
         <v>45139</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="F165" t="s">
-        <v>233</v>
+        <v>209</v>
       </c>
       <c r="G165">
         <v>250</v>
@@ -41952,7 +41952,7 @@
         <v>31</v>
       </c>
       <c r="K165" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L165">
         <v>0</v>
@@ -41961,7 +41961,7 @@
         <v>0</v>
       </c>
       <c r="N165" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="O165">
         <v>0</v>
@@ -42021,7 +42021,7 @@
         <v>0</v>
       </c>
       <c r="AH165" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AI165">
         <v>0</v>
@@ -42176,13 +42176,13 @@
         <v>45139</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>234</v>
+        <v>210</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F166" t="s">
-        <v>235</v>
+        <v>211</v>
       </c>
       <c r="G166">
         <v>250</v>
@@ -42421,13 +42421,13 @@
         <v>45139</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>234</v>
+        <v>210</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>192</v>
+        <v>168</v>
       </c>
       <c r="F167" t="s">
-        <v>244</v>
+        <v>220</v>
       </c>
       <c r="G167">
         <v>250</v>
@@ -42666,13 +42666,13 @@
         <v>45139</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>236</v>
+        <v>212</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>237</v>
+        <v>213</v>
       </c>
       <c r="F168" t="s">
-        <v>238</v>
+        <v>214</v>
       </c>
       <c r="G168">
         <v>250</v>
@@ -42687,7 +42687,7 @@
         <v>31</v>
       </c>
       <c r="K168" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L168" s="2">
         <v>0</v>
@@ -42696,7 +42696,7 @@
         <v>34</v>
       </c>
       <c r="N168" s="2" t="s">
-        <v>214</v>
+        <v>190</v>
       </c>
       <c r="O168" s="2" t="s">
         <v>35</v>
@@ -42911,13 +42911,13 @@
         <v>45139</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>236</v>
+        <v>212</v>
       </c>
       <c r="D169" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="F169" t="s">
-        <v>239</v>
+        <v>215</v>
       </c>
       <c r="G169">
         <v>250</v>
@@ -42932,7 +42932,7 @@
         <v>31</v>
       </c>
       <c r="K169" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L169" s="2">
         <v>0</v>
@@ -42941,7 +42941,7 @@
         <v>34</v>
       </c>
       <c r="N169" s="2" t="s">
-        <v>214</v>
+        <v>190</v>
       </c>
       <c r="O169" s="2" t="s">
         <v>35</v>
@@ -43156,13 +43156,13 @@
         <v>45139</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>236</v>
+        <v>212</v>
       </c>
       <c r="D170" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
       <c r="F170" t="s">
-        <v>245</v>
+        <v>221</v>
       </c>
       <c r="G170">
         <v>250</v>
@@ -43177,7 +43177,7 @@
         <v>31</v>
       </c>
       <c r="K170" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L170" s="2">
         <v>0</v>
@@ -43186,7 +43186,7 @@
         <v>34</v>
       </c>
       <c r="N170" s="2" t="s">
-        <v>214</v>
+        <v>190</v>
       </c>
       <c r="O170" s="2" t="s">
         <v>35</v>
@@ -43401,10 +43401,10 @@
         <v>45139</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>241</v>
+        <v>217</v>
       </c>
       <c r="F171" t="s">
-        <v>246</v>
+        <v>222</v>
       </c>
       <c r="G171">
         <v>170</v>
@@ -43428,7 +43428,7 @@
         <v>0</v>
       </c>
       <c r="N171" s="2" t="s">
-        <v>214</v>
+        <v>190</v>
       </c>
       <c r="O171" s="2">
         <v>0</v>
@@ -43643,10 +43643,10 @@
         <v>45139</v>
       </c>
       <c r="C172" t="s">
-        <v>242</v>
+        <v>218</v>
       </c>
       <c r="F172" t="s">
-        <v>246</v>
+        <v>222</v>
       </c>
       <c r="G172">
         <v>170</v>
@@ -43885,10 +43885,10 @@
         <v>45139</v>
       </c>
       <c r="C173" t="s">
-        <v>243</v>
+        <v>219</v>
       </c>
       <c r="F173" t="s">
-        <v>246</v>
+        <v>222</v>
       </c>
       <c r="G173">
         <v>170</v>
@@ -44125,13 +44125,14 @@
     <hyperlink ref="F159" r:id="rId1" xr:uid="{2EBCD065-C0A9-4D0D-974B-0ABD6971AC2C}"/>
     <hyperlink ref="F39" r:id="rId2" xr:uid="{93300645-12C2-4500-B601-CC5EA36EE083}"/>
     <hyperlink ref="F10" r:id="rId3" xr:uid="{8AA8E1B1-DE7C-4056-A2A2-6DACCBCF8316}"/>
-    <hyperlink ref="F24" r:id="rId4" xr:uid="{44C2B535-F755-42A7-87CF-80F1D4EDA9E5}"/>
+    <hyperlink ref="F24" r:id="rId4" display="https://ductair.github.io/ductaironline/Drawings/TCC/COTE/B/1'.jpg" xr:uid="{44C2B535-F755-42A7-87CF-80F1D4EDA9E5}"/>
     <hyperlink ref="F124" r:id="rId5" xr:uid="{A44C4CDF-411A-4EE3-AFD9-E549429DC73C}"/>
     <hyperlink ref="F127" r:id="rId6" xr:uid="{9891D545-5BE7-4162-9F82-99F187AE80DF}"/>
     <hyperlink ref="F134" r:id="rId7" xr:uid="{CF10C34F-1DC6-4E6A-818B-A1D47625BFD4}"/>
     <hyperlink ref="F137" r:id="rId8" xr:uid="{C4BFBD49-530E-449E-B29C-6619C4A43276}"/>
+    <hyperlink ref="F4" r:id="rId9" xr:uid="{16353D1E-1B5D-470D-B307-8D2218647691}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="57" fitToHeight="0" orientation="landscape" r:id="rId9"/>
+  <pageSetup paperSize="9" scale="57" fitToHeight="0" orientation="landscape" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
maj lien trc centrée et ajout cotes verticales
</commit_message>
<xml_diff>
--- a/Remote/Commun/dist_liens.xlsx
+++ b/Remote/Commun/dist_liens.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Mickaël\Documents\GitHub\ductaironline\ductaironline\Remote\Commun\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Mickaël\Documents\GitHub\ductaironline\Remote\Commun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC892DC7-FB18-4763-BC50-C94D47B492F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E26CCA-1BA9-4F2F-97C1-748E2FC11F4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{10E80606-BDFD-48EA-859F-8B282D217FD1}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3465" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3465" uniqueCount="264">
   <si>
     <t>id</t>
   </si>
@@ -829,6 +829,9 @@
   <si>
     <t>https://ductair.github.io/ductaironline/Drawings/AUTRES/404.jpg</t>
   </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Drawings/TRC/FACE/AØ/0.jpg</t>
+  </si>
 </sst>
 </file>
 
@@ -1240,8 +1243,8 @@
   <dimension ref="A1:CD175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B175"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15470,8 +15473,8 @@
       <c r="E58" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F58" t="s">
-        <v>89</v>
+      <c r="F58" s="8" t="s">
+        <v>263</v>
       </c>
       <c r="G58">
         <v>120</v>
@@ -44636,8 +44639,9 @@
     <hyperlink ref="F4" r:id="rId9" xr:uid="{16353D1E-1B5D-470D-B307-8D2218647691}"/>
     <hyperlink ref="F165" r:id="rId10" xr:uid="{B2839A20-3FC5-49C4-A010-C20261BE5986}"/>
     <hyperlink ref="F175" r:id="rId11" xr:uid="{B0B01E66-2991-40C6-9A40-7D161D71D2A9}"/>
+    <hyperlink ref="F58" r:id="rId12" xr:uid="{366D18FC-0AC7-4944-8D7D-3BE1139D289A}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="57" fitToHeight="0" orientation="landscape" r:id="rId12"/>
+  <pageSetup paperSize="9" scale="57" fitToHeight="0" orientation="landscape" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>